<commit_message>
up to date labels
</commit_message>
<xml_diff>
--- a/Adelaide_stats.xlsx
+++ b/Adelaide_stats.xlsx
@@ -12976,7 +12976,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Goal Assists</t>
+          <t>Goal Assists1</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -17393,7 +17393,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Clearances</t>
+          <t>Clearances1</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -18024,7 +18024,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Clangers</t>
+          <t>Clangers1</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -18655,7 +18655,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Rebound 50s</t>
+          <t>Rebound 50s1</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -30013,7 +30013,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Clangers</t>
+          <t>Clangers2</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -31906,7 +31906,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Clearances</t>
+          <t>Clearances2</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -32537,7 +32537,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Rebound 50s</t>
+          <t>Rebound 50s2</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -34430,7 +34430,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Goals Assists</t>
+          <t>Goals Assists2</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -35692,7 +35692,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Kicks (every)</t>
+          <t>Kicks (O)</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -36323,7 +36323,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Handballs (row)</t>
+          <t>Handballs (O)</t>
         </is>
       </c>
       <c r="B58" t="n">
@@ -36954,7 +36954,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Disposals (from)</t>
+          <t>Disposals (O)</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -37585,7 +37585,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Kick to HB Ratio (kicks)</t>
+          <t>Kick to HB Ratio (O)</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -38216,7 +38216,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Marks (below)</t>
+          <t>Marks (O)</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -38847,7 +38847,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Tackles(is against)</t>
+          <t>Tackles(O)</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -39478,7 +39478,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Hitouts</t>
+          <t>Hitouts(O)</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -40109,7 +40109,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Frees For</t>
+          <t>Frees For(O)</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -40740,7 +40740,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Frees Against</t>
+          <t>Frees Against(O)</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -41371,7 +41371,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Goals Kicked</t>
+          <t>Goals Kicked(O)</t>
         </is>
       </c>
       <c r="B66" t="n">
@@ -42002,7 +42002,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Goal Assists</t>
+          <t>Goal Assists1(O)</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -42633,7 +42633,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Behinds Kicked</t>
+          <t>Behinds Kicked(O)</t>
         </is>
       </c>
       <c r="B68" t="n">
@@ -43264,7 +43264,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Rushed Behinds</t>
+          <t>Rushed Behinds(O)</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -43895,7 +43895,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Scoring Shots</t>
+          <t>Scoring Shots(O)</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -44526,7 +44526,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Conversion %</t>
+          <t>Conversion %(O)</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -45157,7 +45157,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Disposals Per Goal</t>
+          <t>Disposals Per Goal(O)</t>
         </is>
       </c>
       <c r="B72" t="n">
@@ -45788,7 +45788,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Disposals Per Scoring Shot</t>
+          <t>Disposals Per Scoring Shot(O)</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -46419,7 +46419,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Clearances</t>
+          <t>Clearances1(O)</t>
         </is>
       </c>
       <c r="B74" t="n">
@@ -47050,7 +47050,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Clangers</t>
+          <t>Clangers1(O)</t>
         </is>
       </c>
       <c r="B75" t="n">
@@ -47681,7 +47681,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Rebound 50s</t>
+          <t>Rebound 50s1(O)</t>
         </is>
       </c>
       <c r="B76" t="n">
@@ -48312,7 +48312,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Inside 50s</t>
+          <t>Inside 50s(O)</t>
         </is>
       </c>
       <c r="B77" t="n">
@@ -48943,7 +48943,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>In50s Per Scoring Shot</t>
+          <t>In50s Per Scoring Shot(O)</t>
         </is>
       </c>
       <c r="B78" t="n">
@@ -49574,7 +49574,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>In50s Per Goal</t>
+          <t>In50s Per Goal(O)</t>
         </is>
       </c>
       <c r="B79" t="n">
@@ -50205,7 +50205,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>% In50s Score</t>
+          <t>% In50s Score(O)</t>
         </is>
       </c>
       <c r="B80" t="n">
@@ -50836,7 +50836,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>% In50s Goal</t>
+          <t>% In50s Goal(O)</t>
         </is>
       </c>
       <c r="B81" t="n">
@@ -51467,7 +51467,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Height</t>
+          <t>Height(O)</t>
         </is>
       </c>
       <c r="B82" t="n">
@@ -52098,7 +52098,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Weight</t>
+          <t>Weight(O)</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -52729,7 +52729,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Age</t>
+          <t>Age(O)</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -53360,7 +53360,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Av Games</t>
+          <t>Av Games(O)</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -53991,7 +53991,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>&lt;50 Games</t>
+          <t>&lt;50 Games(O)</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -54622,7 +54622,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>50-99 Games</t>
+          <t>50-99 Games(O)</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -55253,7 +55253,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>100-149 Games</t>
+          <t>100-149 Games(O)</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -55884,7 +55884,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>&gt;150 Games</t>
+          <t>&gt;150 Games(O)</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -56515,7 +56515,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Contested Poss</t>
+          <t>Contested Poss(O)</t>
         </is>
       </c>
       <c r="B90" t="n">
@@ -57146,7 +57146,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Uncontested Poss</t>
+          <t>Uncontested Poss(O)</t>
         </is>
       </c>
       <c r="B91" t="n">
@@ -57777,7 +57777,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Effective Disposals</t>
+          <t>Effective Disposals(O)</t>
         </is>
       </c>
       <c r="B92" t="n">
@@ -58408,7 +58408,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Disposal Efficiency</t>
+          <t>Disposal Efficiency(O)</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -59039,7 +59039,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Clangers</t>
+          <t>Clangers2(O)</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -59670,7 +59670,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Contested Marks</t>
+          <t>Contested Marks(O)</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -60301,7 +60301,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Marks Inside 50</t>
+          <t>Marks Inside 50(O)</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -60932,7 +60932,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Clearances</t>
+          <t>Clearances2(O)</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -61563,7 +61563,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Rebound 50s</t>
+          <t>Rebound 50s2(O)</t>
         </is>
       </c>
       <c r="B98" t="n">
@@ -62194,7 +62194,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>1%ers</t>
+          <t>1%ers(O)</t>
         </is>
       </c>
       <c r="B99" t="n">
@@ -62825,7 +62825,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Bounces</t>
+          <t>Bounces(O)</t>
         </is>
       </c>
       <c r="B100" t="n">
@@ -63456,7 +63456,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Goals Assists</t>
+          <t>Goals Assists2(O)</t>
         </is>
       </c>
       <c r="B101" t="n">
@@ -64087,7 +64087,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Goal Assist %</t>
+          <t>Goal Assist %(O)</t>
         </is>
       </c>
       <c r="B102" t="n">

</xml_diff>

<commit_message>
updated with round 4 results 2020
</commit_message>
<xml_diff>
--- a/Adelaide_stats.xlsx
+++ b/Adelaide_stats.xlsx
@@ -4,13 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
 </workbook>
 </file>
 
@@ -59,31 +59,31 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -377,18 +377,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HE102"/>
+  <dimension ref="A1:HF102"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="GZ1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="HA23" activeCellId="0" pane="topLeft" sqref="HA23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col width="8.529999999999999" customWidth="1" style="1" min="1" max="1025"/>
+    <col customWidth="1" max="1025" min="1" style="1" width="8.529999999999999"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="1" s="2">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Match_ID</t>
@@ -1027,11 +1027,14 @@
       <c r="HD1" s="1" t="n">
         <v>10130</v>
       </c>
-      <c r="HE1" t="n">
+      <c r="HE1" s="1" t="n">
         <v>10141</v>
       </c>
+      <c r="HF1" t="n">
+        <v>10150</v>
+      </c>
     </row>
-    <row r="2" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="2" s="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Year</t>
@@ -1670,11 +1673,14 @@
       <c r="HD2" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="HE2" t="n">
+      <c r="HE2" s="1" t="n">
         <v>2020</v>
       </c>
+      <c r="HF2" t="n">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="3" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="3" s="2">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Round</t>
@@ -2313,11 +2319,14 @@
       <c r="HD3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HE3" t="n">
+      <c r="HE3" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="HF3" t="n">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="4" s="2">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>H/A?</t>
@@ -2956,11 +2965,14 @@
       <c r="HD4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HE4" t="n">
+      <c r="HE4" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="HF4" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="5" s="2">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>H/A Win?</t>
@@ -3599,11 +3611,14 @@
       <c r="HD5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HE5" t="n">
+      <c r="HE5" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="HF5" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="6" s="2">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Points For</t>
@@ -4242,11 +4257,14 @@
       <c r="HD6" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="HE6" t="n">
+      <c r="HE6" s="1" t="n">
         <v>29</v>
       </c>
+      <c r="HF6" t="n">
+        <v>46</v>
+      </c>
     </row>
-    <row r="7" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="7" s="2">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Points Against</t>
@@ -4885,11 +4903,14 @@
       <c r="HD7" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="HE7" t="n">
+      <c r="HE7" s="1" t="n">
         <v>82</v>
       </c>
+      <c r="HF7" t="n">
+        <v>83</v>
+      </c>
     </row>
-    <row r="8" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="8" s="2">
       <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Margin</t>
@@ -5528,11 +5549,14 @@
       <c r="HD8" s="1" t="n">
         <v>-75</v>
       </c>
-      <c r="HE8" t="n">
+      <c r="HE8" s="1" t="n">
         <v>-53</v>
       </c>
+      <c r="HF8" t="n">
+        <v>-37</v>
+      </c>
     </row>
-    <row r="9" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="9" s="2">
       <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Team Won? (1=W, 0=L)</t>
@@ -6171,11 +6195,14 @@
       <c r="HD9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HE9" t="n">
+      <c r="HE9" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="HF9" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="10" s="2">
       <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Team_against_ID</t>
@@ -6814,11 +6841,14 @@
       <c r="HD10" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HE10" t="n">
+      <c r="HE10" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="HF10" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row r="11" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="11" s="2">
       <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Kicks</t>
@@ -7457,11 +7487,14 @@
       <c r="HD11" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="HE11" t="n">
+      <c r="HE11" s="1" t="n">
         <v>145</v>
       </c>
+      <c r="HF11" t="n">
+        <v>162</v>
+      </c>
     </row>
-    <row r="12" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="12" s="2">
       <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Handballs</t>
@@ -8100,11 +8133,14 @@
       <c r="HD12" s="1" t="n">
         <v>121</v>
       </c>
-      <c r="HE12" t="n">
+      <c r="HE12" s="1" t="n">
         <v>105</v>
       </c>
+      <c r="HF12" t="n">
+        <v>70</v>
+      </c>
     </row>
-    <row r="13" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="13" s="2">
       <c r="A13" s="1" t="inlineStr">
         <is>
           <t>Disposals</t>
@@ -8743,11 +8779,14 @@
       <c r="HD13" s="1" t="n">
         <v>259</v>
       </c>
-      <c r="HE13" t="n">
+      <c r="HE13" s="1" t="n">
         <v>250</v>
       </c>
+      <c r="HF13" t="n">
+        <v>232</v>
+      </c>
     </row>
-    <row r="14" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="14" s="2">
       <c r="A14" s="1" t="inlineStr">
         <is>
           <t>Kick to HB Ratio</t>
@@ -9386,11 +9425,14 @@
       <c r="HD14" s="1" t="n">
         <v>1.14</v>
       </c>
-      <c r="HE14" t="n">
+      <c r="HE14" s="1" t="n">
         <v>1.38</v>
       </c>
+      <c r="HF14" t="n">
+        <v>2.31</v>
+      </c>
     </row>
-    <row r="15" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="15" s="2">
       <c r="A15" s="1" t="inlineStr">
         <is>
           <t>Marks</t>
@@ -10029,11 +10071,14 @@
       <c r="HD15" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="HE15" t="n">
+      <c r="HE15" s="1" t="n">
         <v>56</v>
       </c>
+      <c r="HF15" t="n">
+        <v>71</v>
+      </c>
     </row>
-    <row r="16" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="16" s="2">
       <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Tackles</t>
@@ -10672,11 +10717,14 @@
       <c r="HD16" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="HE16" t="n">
+      <c r="HE16" s="1" t="n">
         <v>57</v>
       </c>
+      <c r="HF16" t="n">
+        <v>55</v>
+      </c>
     </row>
-    <row r="17" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="17" s="2">
       <c r="A17" s="1" t="inlineStr">
         <is>
           <t>Hitouts</t>
@@ -11315,11 +11363,14 @@
       <c r="HD17" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HE17" t="n">
+      <c r="HE17" s="1" t="n">
         <v>39</v>
       </c>
+      <c r="HF17" t="n">
+        <v>24</v>
+      </c>
     </row>
-    <row r="18" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="18" s="2">
       <c r="A18" s="1" t="inlineStr">
         <is>
           <t>Frees For</t>
@@ -11958,11 +12009,14 @@
       <c r="HD18" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HE18" t="n">
+      <c r="HE18" s="1" t="n">
         <v>26</v>
       </c>
+      <c r="HF18" t="n">
+        <v>17</v>
+      </c>
     </row>
-    <row r="19" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="19" s="2">
       <c r="A19" s="1" t="inlineStr">
         <is>
           <t>Frees Against</t>
@@ -12601,11 +12655,14 @@
       <c r="HD19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="HE19" t="n">
+      <c r="HE19" s="1" t="n">
         <v>16</v>
       </c>
+      <c r="HF19" t="n">
+        <v>20</v>
+      </c>
     </row>
-    <row r="20" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="20" s="2">
       <c r="A20" s="1" t="inlineStr">
         <is>
           <t>Goals Kicked</t>
@@ -13244,11 +13301,14 @@
       <c r="HD20" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HE20" t="n">
+      <c r="HE20" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="HF20" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row r="21" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="21" s="2">
       <c r="A21" s="1" t="inlineStr">
         <is>
           <t>Goal Assists1</t>
@@ -13887,11 +13947,14 @@
       <c r="HD21" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HE21" t="n">
+      <c r="HE21" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HF21" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row r="22" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="22" s="2">
       <c r="A22" s="1" t="inlineStr">
         <is>
           <t>Behinds Kicked</t>
@@ -14530,11 +14593,14 @@
       <c r="HD22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HE22" t="n">
+      <c r="HE22" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="HF22" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="23" s="2">
       <c r="A23" s="1" t="inlineStr">
         <is>
           <t>Rushed Behinds</t>
@@ -15173,11 +15239,14 @@
       <c r="HD23" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HE23" t="n">
+      <c r="HE23" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HF23" t="n">
+        <v>3</v>
+      </c>
     </row>
-    <row r="24" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="24" s="2">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>Scoring Shots</t>
@@ -15816,11 +15885,14 @@
       <c r="HD24" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HE24" t="n">
+      <c r="HE24" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="HF24" t="n">
+        <v>11</v>
+      </c>
     </row>
-    <row r="25" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="25" s="2">
       <c r="A25" s="1" t="inlineStr">
         <is>
           <t>Conversion %</t>
@@ -16459,11 +16531,14 @@
       <c r="HD25" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HE25" t="n">
+      <c r="HE25" s="1" t="n">
         <v>44.4</v>
       </c>
+      <c r="HF25" t="n">
+        <v>63.6</v>
+      </c>
     </row>
-    <row r="26" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="26" s="2">
       <c r="A26" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Goal</t>
@@ -17102,11 +17177,14 @@
       <c r="HD26" s="1" t="n">
         <v>51.8</v>
       </c>
-      <c r="HE26" t="n">
+      <c r="HE26" s="1" t="n">
         <v>62.5</v>
       </c>
+      <c r="HF26" t="n">
+        <v>33.14</v>
+      </c>
     </row>
-    <row r="27" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="27" s="2">
       <c r="A27" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Scoring Shot</t>
@@ -17745,11 +17823,14 @@
       <c r="HD27" s="1" t="n">
         <v>25.9</v>
       </c>
-      <c r="HE27" t="n">
+      <c r="HE27" s="1" t="n">
         <v>27.78</v>
       </c>
+      <c r="HF27" t="n">
+        <v>21.09</v>
+      </c>
     </row>
-    <row r="28" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="28" s="2">
       <c r="A28" s="1" t="inlineStr">
         <is>
           <t>Clearances1</t>
@@ -18388,11 +18469,14 @@
       <c r="HD28" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HE28" t="n">
+      <c r="HE28" s="1" t="n">
         <v>25</v>
       </c>
+      <c r="HF28" t="n">
+        <v>22</v>
+      </c>
     </row>
-    <row r="29" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="29" s="2">
       <c r="A29" s="1" t="inlineStr">
         <is>
           <t>Clangers1</t>
@@ -19031,11 +19115,14 @@
       <c r="HD29" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HE29" t="n">
+      <c r="HE29" s="1" t="n">
         <v>46</v>
       </c>
+      <c r="HF29" t="n">
+        <v>50</v>
+      </c>
     </row>
-    <row r="30" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="30" s="2">
       <c r="A30" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s1</t>
@@ -19674,11 +19761,14 @@
       <c r="HD30" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="HE30" t="n">
+      <c r="HE30" s="1" t="n">
         <v>43</v>
       </c>
+      <c r="HF30" t="n">
+        <v>46</v>
+      </c>
     </row>
-    <row r="31" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="31" s="2">
       <c r="A31" s="1" t="inlineStr">
         <is>
           <t>Inside 50s</t>
@@ -20317,11 +20407,14 @@
       <c r="HD31" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HE31" t="n">
+      <c r="HE31" s="1" t="n">
         <v>28</v>
       </c>
+      <c r="HF31" t="n">
+        <v>28</v>
+      </c>
     </row>
-    <row r="32" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="32" s="2">
       <c r="A32" s="1" t="inlineStr">
         <is>
           <t>In50s Per Scoring Shot</t>
@@ -20960,11 +21053,14 @@
       <c r="HD32" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HE32" t="n">
+      <c r="HE32" s="1" t="n">
         <v>3.11</v>
       </c>
+      <c r="HF32" t="n">
+        <v>2.55</v>
+      </c>
     </row>
-    <row r="33" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="33" s="2">
       <c r="A33" s="1" t="inlineStr">
         <is>
           <t>In50s Per Goal</t>
@@ -21603,11 +21699,14 @@
       <c r="HD33" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HE33" t="n">
+      <c r="HE33" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="HF33" t="n">
+        <v>4</v>
+      </c>
     </row>
-    <row r="34" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="34" s="2">
       <c r="A34" s="1" t="inlineStr">
         <is>
           <t>% In50s Score</t>
@@ -22246,11 +22345,14 @@
       <c r="HD34" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="HE34" t="n">
+      <c r="HE34" s="1" t="n">
         <v>25</v>
       </c>
+      <c r="HF34" t="n">
+        <v>28.6</v>
+      </c>
     </row>
-    <row r="35" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="35" s="2">
       <c r="A35" s="1" t="inlineStr">
         <is>
           <t>% In50s Goal</t>
@@ -22889,11 +22991,14 @@
       <c r="HD35" s="1" t="n">
         <v>16.7</v>
       </c>
-      <c r="HE35" t="n">
+      <c r="HE35" s="1" t="n">
         <v>14.3</v>
       </c>
+      <c r="HF35" t="n">
+        <v>25</v>
+      </c>
     </row>
-    <row r="36" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="36" s="2">
       <c r="A36" s="1" t="inlineStr">
         <is>
           <t>Height</t>
@@ -23532,11 +23637,14 @@
       <c r="HD36" s="1" t="n">
         <v>187.2</v>
       </c>
-      <c r="HE36" t="n">
+      <c r="HE36" s="1" t="n">
         <v>187.3</v>
       </c>
+      <c r="HF36" t="n">
+        <v>187.9</v>
+      </c>
     </row>
-    <row r="37" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="37" s="2">
       <c r="A37" s="1" t="inlineStr">
         <is>
           <t>Weight</t>
@@ -24175,11 +24283,14 @@
       <c r="HD37" s="1" t="n">
         <v>86.3</v>
       </c>
-      <c r="HE37" t="n">
+      <c r="HE37" s="1" t="n">
         <v>85.8</v>
       </c>
+      <c r="HF37" t="n">
+        <v>86</v>
+      </c>
     </row>
-    <row r="38" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="38" s="2">
       <c r="A38" s="1" t="inlineStr">
         <is>
           <t>Age</t>
@@ -24818,11 +24929,14 @@
       <c r="HD38" s="1" t="n">
         <v>25.8</v>
       </c>
-      <c r="HE38" t="n">
+      <c r="HE38" s="1" t="n">
         <v>25</v>
       </c>
+      <c r="HF38" t="n">
+        <v>24.66</v>
+      </c>
     </row>
-    <row r="39" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="39" s="2">
       <c r="A39" s="1" t="inlineStr">
         <is>
           <t>Av Games</t>
@@ -25461,11 +25575,14 @@
       <c r="HD39" s="1" t="n">
         <v>85.90000000000001</v>
       </c>
-      <c r="HE39" t="n">
+      <c r="HE39" s="1" t="n">
         <v>84</v>
       </c>
+      <c r="HF39" t="n">
+        <v>71</v>
+      </c>
     </row>
-    <row r="40" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="40" s="2">
       <c r="A40" s="1" t="inlineStr">
         <is>
           <t>&lt;50 Games</t>
@@ -26104,11 +26221,14 @@
       <c r="HD40" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HE40" t="n">
+      <c r="HE40" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="HF40" t="n">
+        <v>13</v>
+      </c>
     </row>
-    <row r="41" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="41" s="2">
       <c r="A41" s="1" t="inlineStr">
         <is>
           <t>50-99 Games</t>
@@ -26747,11 +26867,14 @@
       <c r="HD41" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HE41" t="n">
+      <c r="HE41" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HF41" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row r="42" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="42" s="2">
       <c r="A42" s="1" t="inlineStr">
         <is>
           <t>100-149 Games</t>
@@ -27390,11 +27513,14 @@
       <c r="HD42" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HE42" t="n">
+      <c r="HE42" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="HF42" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row r="43" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="43" s="2">
       <c r="A43" s="1" t="inlineStr">
         <is>
           <t>&gt;150 Games</t>
@@ -28033,11 +28159,14 @@
       <c r="HD43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HE43" t="n">
+      <c r="HE43" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="HF43" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row r="44" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="44" s="2">
       <c r="A44" s="1" t="inlineStr">
         <is>
           <t>Contested Poss</t>
@@ -28676,11 +28805,14 @@
       <c r="HD44" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="HE44" t="n">
+      <c r="HE44" s="1" t="n">
         <v>105</v>
       </c>
+      <c r="HF44" t="n">
+        <v>91</v>
+      </c>
     </row>
-    <row r="45" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="45" s="2">
       <c r="A45" s="1" t="inlineStr">
         <is>
           <t>Uncontested Poss</t>
@@ -29319,11 +29451,14 @@
       <c r="HD45" s="1" t="n">
         <v>133</v>
       </c>
-      <c r="HE45" t="n">
+      <c r="HE45" s="1" t="n">
         <v>143</v>
       </c>
+      <c r="HF45" t="n">
+        <v>125</v>
+      </c>
     </row>
-    <row r="46" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="46" s="2">
       <c r="A46" s="1" t="inlineStr">
         <is>
           <t>Effective Disposals</t>
@@ -29962,11 +30097,14 @@
       <c r="HD46" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="HE46" t="n">
+      <c r="HE46" s="1" t="n">
         <v>180</v>
       </c>
+      <c r="HF46" t="n">
+        <v>166</v>
+      </c>
     </row>
-    <row r="47" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="47" s="2">
       <c r="A47" s="1" t="inlineStr">
         <is>
           <t>Disposal Efficiency</t>
@@ -30605,11 +30743,14 @@
       <c r="HD47" s="1" t="n">
         <v>62.5</v>
       </c>
-      <c r="HE47" t="n">
+      <c r="HE47" s="1" t="n">
         <v>72</v>
       </c>
+      <c r="HF47" t="n">
+        <v>71.59999999999999</v>
+      </c>
     </row>
-    <row r="48" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="48" s="2">
       <c r="A48" s="1" t="inlineStr">
         <is>
           <t>Clangers2</t>
@@ -31248,11 +31389,14 @@
       <c r="HD48" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HE48" t="n">
+      <c r="HE48" s="1" t="n">
         <v>46</v>
       </c>
+      <c r="HF48" t="n">
+        <v>50</v>
+      </c>
     </row>
-    <row r="49" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="49" s="2">
       <c r="A49" s="1" t="inlineStr">
         <is>
           <t>Contested Marks</t>
@@ -31891,11 +32035,14 @@
       <c r="HD49" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HE49" t="n">
+      <c r="HE49" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="HF49" t="n">
+        <v>4</v>
+      </c>
     </row>
-    <row r="50" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="50" s="2">
       <c r="A50" s="1" t="inlineStr">
         <is>
           <t>Marks Inside 50</t>
@@ -32534,11 +32681,14 @@
       <c r="HD50" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HE50" t="n">
+      <c r="HE50" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HF50" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row r="51" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="51" s="2">
       <c r="A51" s="1" t="inlineStr">
         <is>
           <t>Clearances2</t>
@@ -33177,11 +33327,14 @@
       <c r="HD51" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HE51" t="n">
+      <c r="HE51" s="1" t="n">
         <v>25</v>
       </c>
+      <c r="HF51" t="n">
+        <v>22</v>
+      </c>
     </row>
-    <row r="52" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="52" s="2">
       <c r="A52" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s2</t>
@@ -33820,11 +33973,14 @@
       <c r="HD52" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="HE52" t="n">
+      <c r="HE52" s="1" t="n">
         <v>43</v>
       </c>
+      <c r="HF52" t="n">
+        <v>46</v>
+      </c>
     </row>
-    <row r="53" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="53" s="2">
       <c r="A53" s="1" t="inlineStr">
         <is>
           <t>1%ers</t>
@@ -34463,11 +34619,14 @@
       <c r="HD53" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="HE53" t="n">
+      <c r="HE53" s="1" t="n">
         <v>33</v>
       </c>
+      <c r="HF53" t="n">
+        <v>34</v>
+      </c>
     </row>
-    <row r="54" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="54" s="2">
       <c r="A54" s="1" t="inlineStr">
         <is>
           <t>Bounces</t>
@@ -35106,11 +35265,14 @@
       <c r="HD54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HE54" t="n">
+      <c r="HE54" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HF54" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row r="55" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="55" s="2">
       <c r="A55" s="1" t="inlineStr">
         <is>
           <t>Goals Assists2</t>
@@ -35749,11 +35911,14 @@
       <c r="HD55" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HE55" t="n">
+      <c r="HE55" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HF55" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row r="56" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="56" s="2">
       <c r="A56" s="1" t="inlineStr">
         <is>
           <t>Goal Assist %</t>
@@ -36392,11 +36557,14 @@
       <c r="HD56" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="HE56" t="n">
+      <c r="HE56" s="1" t="n">
         <v>50</v>
       </c>
+      <c r="HF56" t="n">
+        <v>71.40000000000001</v>
+      </c>
     </row>
-    <row r="57" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="57" s="2">
       <c r="A57" s="1" t="inlineStr">
         <is>
           <t>Kicks (O)</t>
@@ -37035,11 +37203,14 @@
       <c r="HD57" s="1" t="n">
         <v>226</v>
       </c>
-      <c r="HE57" t="n">
+      <c r="HE57" s="1" t="n">
         <v>195</v>
       </c>
+      <c r="HF57" t="n">
+        <v>199</v>
+      </c>
     </row>
-    <row r="58" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="58" s="2">
       <c r="A58" s="1" t="inlineStr">
         <is>
           <t>Handballs (O)</t>
@@ -37678,11 +37849,14 @@
       <c r="HD58" s="1" t="n">
         <v>137</v>
       </c>
-      <c r="HE58" t="n">
+      <c r="HE58" s="1" t="n">
         <v>123</v>
       </c>
+      <c r="HF58" t="n">
+        <v>86</v>
+      </c>
     </row>
-    <row r="59" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="59" s="2">
       <c r="A59" s="1" t="inlineStr">
         <is>
           <t>Disposals (O)</t>
@@ -38321,11 +38495,14 @@
       <c r="HD59" s="1" t="n">
         <v>363</v>
       </c>
-      <c r="HE59" t="n">
+      <c r="HE59" s="1" t="n">
         <v>318</v>
       </c>
+      <c r="HF59" t="n">
+        <v>285</v>
+      </c>
     </row>
-    <row r="60" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="60" s="2">
       <c r="A60" s="1" t="inlineStr">
         <is>
           <t>Kick to HB Ratio (O)</t>
@@ -38964,11 +39141,14 @@
       <c r="HD60" s="1" t="n">
         <v>1.65</v>
       </c>
-      <c r="HE60" t="n">
+      <c r="HE60" s="1" t="n">
         <v>1.59</v>
       </c>
+      <c r="HF60" t="n">
+        <v>2.31</v>
+      </c>
     </row>
-    <row r="61" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="61" s="2">
       <c r="A61" s="1" t="inlineStr">
         <is>
           <t>Marks (O)</t>
@@ -39607,11 +39787,14 @@
       <c r="HD61" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="HE61" t="n">
+      <c r="HE61" s="1" t="n">
         <v>87</v>
       </c>
+      <c r="HF61" t="n">
+        <v>80</v>
+      </c>
     </row>
-    <row r="62" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="62" s="2">
       <c r="A62" s="1" t="inlineStr">
         <is>
           <t>Tackles(O)</t>
@@ -40250,11 +40433,14 @@
       <c r="HD62" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="HE62" t="n">
+      <c r="HE62" s="1" t="n">
         <v>75</v>
       </c>
+      <c r="HF62" t="n">
+        <v>68</v>
+      </c>
     </row>
-    <row r="63" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="63" s="2">
       <c r="A63" s="1" t="inlineStr">
         <is>
           <t>Hitouts(O)</t>
@@ -40893,11 +41079,14 @@
       <c r="HD63" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="HE63" t="n">
+      <c r="HE63" s="1" t="n">
         <v>27</v>
       </c>
+      <c r="HF63" t="n">
+        <v>29</v>
+      </c>
     </row>
-    <row r="64" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="64" s="2">
       <c r="A64" s="1" t="inlineStr">
         <is>
           <t>Frees For(O)</t>
@@ -41536,11 +41725,14 @@
       <c r="HD64" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="HE64" t="n">
+      <c r="HE64" s="1" t="n">
         <v>16</v>
       </c>
+      <c r="HF64" t="n">
+        <v>20</v>
+      </c>
     </row>
-    <row r="65" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="65" s="2">
       <c r="A65" s="1" t="inlineStr">
         <is>
           <t>Frees Against(O)</t>
@@ -42179,11 +42371,14 @@
       <c r="HD65" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HE65" t="n">
+      <c r="HE65" s="1" t="n">
         <v>26</v>
       </c>
+      <c r="HF65" t="n">
+        <v>17</v>
+      </c>
     </row>
-    <row r="66" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="66" s="2">
       <c r="A66" s="1" t="inlineStr">
         <is>
           <t>Goals Kicked(O)</t>
@@ -42822,11 +43017,14 @@
       <c r="HD66" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="HE66" t="n">
+      <c r="HE66" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="HF66" t="n">
+        <v>10</v>
+      </c>
     </row>
-    <row r="67" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="67" s="2">
       <c r="A67" s="1" t="inlineStr">
         <is>
           <t>Goal Assists1(O)</t>
@@ -43465,11 +43663,14 @@
       <c r="HD67" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HE67" t="n">
+      <c r="HE67" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="HF67" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row r="68" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="68" s="2">
       <c r="A68" s="1" t="inlineStr">
         <is>
           <t>Behinds Kicked(O)</t>
@@ -44108,11 +44309,14 @@
       <c r="HD68" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HE68" t="n">
+      <c r="HE68" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="HF68" t="n">
+        <v>22</v>
+      </c>
     </row>
-    <row r="69" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="69" s="2">
       <c r="A69" s="1" t="inlineStr">
         <is>
           <t>Rushed Behinds(O)</t>
@@ -44751,11 +44955,14 @@
       <c r="HD69" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HE69" t="n">
+      <c r="HE69" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="HF69" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row r="70" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="70" s="2">
       <c r="A70" s="1" t="inlineStr">
         <is>
           <t>Scoring Shots(O)</t>
@@ -45394,11 +45601,14 @@
       <c r="HD70" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HE70" t="n">
+      <c r="HE70" s="1" t="n">
         <v>22</v>
       </c>
+      <c r="HF70" t="n">
+        <v>33</v>
+      </c>
     </row>
-    <row r="71" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="71" s="2">
       <c r="A71" s="1" t="inlineStr">
         <is>
           <t>Conversion %(O)</t>
@@ -46037,11 +46247,14 @@
       <c r="HD71" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="HE71" t="n">
+      <c r="HE71" s="1" t="n">
         <v>54.5</v>
       </c>
+      <c r="HF71" t="n">
+        <v>30.3</v>
+      </c>
     </row>
-    <row r="72" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="72" s="2">
       <c r="A72" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Goal(O)</t>
@@ -46680,11 +46893,14 @@
       <c r="HD72" s="1" t="n">
         <v>21.35</v>
       </c>
-      <c r="HE72" t="n">
+      <c r="HE72" s="1" t="n">
         <v>26.5</v>
       </c>
+      <c r="HF72" t="n">
+        <v>28.5</v>
+      </c>
     </row>
-    <row r="73" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="73" s="2">
       <c r="A73" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Scoring Shot(O)</t>
@@ -47323,11 +47539,14 @@
       <c r="HD73" s="1" t="n">
         <v>14.52</v>
       </c>
-      <c r="HE73" t="n">
+      <c r="HE73" s="1" t="n">
         <v>14.45</v>
       </c>
+      <c r="HF73" t="n">
+        <v>8.640000000000001</v>
+      </c>
     </row>
-    <row r="74" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="74" s="2">
       <c r="A74" s="1" t="inlineStr">
         <is>
           <t>Clearances1(O)</t>
@@ -47966,11 +48185,14 @@
       <c r="HD74" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="HE74" t="n">
+      <c r="HE74" s="1" t="n">
         <v>38</v>
       </c>
+      <c r="HF74" t="n">
+        <v>31</v>
+      </c>
     </row>
-    <row r="75" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="75" s="2">
       <c r="A75" s="1" t="inlineStr">
         <is>
           <t>Clangers1(O)</t>
@@ -48609,11 +48831,14 @@
       <c r="HD75" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="HE75" t="n">
+      <c r="HE75" s="1" t="n">
         <v>61</v>
       </c>
+      <c r="HF75" t="n">
+        <v>32</v>
+      </c>
     </row>
-    <row r="76" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="76" s="2">
       <c r="A76" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s1(O)</t>
@@ -49252,11 +49477,14 @@
       <c r="HD76" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HE76" t="n">
+      <c r="HE76" s="1" t="n">
         <v>24</v>
       </c>
+      <c r="HF76" t="n">
+        <v>21</v>
+      </c>
     </row>
-    <row r="77" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="77" s="2">
       <c r="A77" s="1" t="inlineStr">
         <is>
           <t>Inside 50s(O)</t>
@@ -49895,11 +50123,14 @@
       <c r="HD77" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="HE77" t="n">
+      <c r="HE77" s="1" t="n">
         <v>56</v>
       </c>
+      <c r="HF77" t="n">
+        <v>60</v>
+      </c>
     </row>
-    <row r="78" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="78" s="2">
       <c r="A78" s="1" t="inlineStr">
         <is>
           <t>In50s Per Scoring Shot(O)</t>
@@ -50538,11 +50769,14 @@
       <c r="HD78" s="1" t="n">
         <v>2.28</v>
       </c>
-      <c r="HE78" t="n">
+      <c r="HE78" s="1" t="n">
         <v>2.55</v>
       </c>
+      <c r="HF78" t="n">
+        <v>1.82</v>
+      </c>
     </row>
-    <row r="79" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="79" s="2">
       <c r="A79" s="1" t="inlineStr">
         <is>
           <t>In50s Per Goal(O)</t>
@@ -51181,11 +51415,14 @@
       <c r="HD79" s="1" t="n">
         <v>3.35</v>
       </c>
-      <c r="HE79" t="n">
+      <c r="HE79" s="1" t="n">
         <v>4.67</v>
       </c>
+      <c r="HF79" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row r="80" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="80" s="2">
       <c r="A80" s="1" t="inlineStr">
         <is>
           <t>% In50s Score(O)</t>
@@ -51824,11 +52061,14 @@
       <c r="HD80" s="1" t="n">
         <v>36.8</v>
       </c>
-      <c r="HE80" t="n">
+      <c r="HE80" s="1" t="n">
         <v>37.5</v>
       </c>
+      <c r="HF80" t="n">
+        <v>53.3</v>
+      </c>
     </row>
-    <row r="81" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="81" s="2">
       <c r="A81" s="1" t="inlineStr">
         <is>
           <t>% In50s Goal(O)</t>
@@ -52467,11 +52707,14 @@
       <c r="HD81" s="1" t="n">
         <v>29.8</v>
       </c>
-      <c r="HE81" t="n">
+      <c r="HE81" s="1" t="n">
         <v>21.4</v>
       </c>
+      <c r="HF81" t="n">
+        <v>16.7</v>
+      </c>
     </row>
-    <row r="82" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="82" s="2">
       <c r="A82" s="1" t="inlineStr">
         <is>
           <t>Height(O)</t>
@@ -53110,11 +53353,14 @@
       <c r="HD82" s="1" t="n">
         <v>188.5</v>
       </c>
-      <c r="HE82" t="n">
+      <c r="HE82" s="1" t="n">
         <v>186.9</v>
       </c>
+      <c r="HF82" t="n">
+        <v>188.9</v>
+      </c>
     </row>
-    <row r="83" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="83" s="2">
       <c r="A83" s="1" t="inlineStr">
         <is>
           <t>Weight(O)</t>
@@ -53753,11 +53999,14 @@
       <c r="HD83" s="1" t="n">
         <v>84.59999999999999</v>
       </c>
-      <c r="HE83" t="n">
+      <c r="HE83" s="1" t="n">
         <v>85.3</v>
       </c>
+      <c r="HF83" t="n">
+        <v>89</v>
+      </c>
     </row>
-    <row r="84" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="84" s="2">
       <c r="A84" s="1" t="inlineStr">
         <is>
           <t>Age(O)</t>
@@ -54396,11 +54645,14 @@
       <c r="HD84" s="1" t="n">
         <v>26.49</v>
       </c>
-      <c r="HE84" t="n">
+      <c r="HE84" s="1" t="n">
         <v>24.33</v>
       </c>
+      <c r="HF84" t="n">
+        <v>25.66</v>
+      </c>
     </row>
-    <row r="85" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="85" s="2">
       <c r="A85" s="1" t="inlineStr">
         <is>
           <t>Av Games(O)</t>
@@ -55039,11 +55291,14 @@
       <c r="HD85" s="1" t="n">
         <v>116.6</v>
       </c>
-      <c r="HE85" t="n">
+      <c r="HE85" s="1" t="n">
         <v>74.2</v>
       </c>
+      <c r="HF85" t="n">
+        <v>98.5</v>
+      </c>
     </row>
-    <row r="86" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="86" s="2">
       <c r="A86" s="1" t="inlineStr">
         <is>
           <t>&lt;50 Games(O)</t>
@@ -55682,11 +55937,14 @@
       <c r="HD86" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HE86" t="n">
+      <c r="HE86" s="1" t="n">
         <v>12</v>
       </c>
+      <c r="HF86" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row r="87" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="87" s="2">
       <c r="A87" s="1" t="inlineStr">
         <is>
           <t>50-99 Games(O)</t>
@@ -56325,11 +56583,14 @@
       <c r="HD87" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HE87" t="n">
+      <c r="HE87" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HF87" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row r="88" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="88" s="2">
       <c r="A88" s="1" t="inlineStr">
         <is>
           <t>100-149 Games(O)</t>
@@ -56968,11 +57229,14 @@
       <c r="HD88" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HE88" t="n">
+      <c r="HE88" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="HF88" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row r="89" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="89" s="2">
       <c r="A89" s="1" t="inlineStr">
         <is>
           <t>&gt;150 Games(O)</t>
@@ -57611,11 +57875,14 @@
       <c r="HD89" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HE89" t="n">
+      <c r="HE89" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="HF89" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row r="90" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="90" s="2">
       <c r="A90" s="1" t="inlineStr">
         <is>
           <t>Contested Poss(O)</t>
@@ -58254,11 +58521,14 @@
       <c r="HD90" s="1" t="n">
         <v>138</v>
       </c>
-      <c r="HE90" t="n">
+      <c r="HE90" s="1" t="n">
         <v>122</v>
       </c>
+      <c r="HF90" t="n">
+        <v>131</v>
+      </c>
     </row>
-    <row r="91" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="91" s="2">
       <c r="A91" s="1" t="inlineStr">
         <is>
           <t>Uncontested Poss(O)</t>
@@ -58897,11 +59167,14 @@
       <c r="HD91" s="1" t="n">
         <v>225</v>
       </c>
-      <c r="HE91" t="n">
+      <c r="HE91" s="1" t="n">
         <v>192</v>
       </c>
+      <c r="HF91" t="n">
+        <v>145</v>
+      </c>
     </row>
-    <row r="92" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="92" s="2">
       <c r="A92" s="1" t="inlineStr">
         <is>
           <t>Effective Disposals(O)</t>
@@ -59540,11 +59813,14 @@
       <c r="HD92" s="1" t="n">
         <v>268</v>
       </c>
-      <c r="HE92" t="n">
+      <c r="HE92" s="1" t="n">
         <v>227</v>
       </c>
+      <c r="HF92" t="n">
+        <v>190</v>
+      </c>
     </row>
-    <row r="93" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="93" s="2">
       <c r="A93" s="1" t="inlineStr">
         <is>
           <t>Disposal Efficiency(O)</t>
@@ -60183,11 +60459,14 @@
       <c r="HD93" s="1" t="n">
         <v>73.8</v>
       </c>
-      <c r="HE93" t="n">
+      <c r="HE93" s="1" t="n">
         <v>71.40000000000001</v>
       </c>
+      <c r="HF93" t="n">
+        <v>66.7</v>
+      </c>
     </row>
-    <row r="94" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="94" s="2">
       <c r="A94" s="1" t="inlineStr">
         <is>
           <t>Clangers2(O)</t>
@@ -60826,11 +61105,14 @@
       <c r="HD94" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="HE94" t="n">
+      <c r="HE94" s="1" t="n">
         <v>61</v>
       </c>
+      <c r="HF94" t="n">
+        <v>32</v>
+      </c>
     </row>
-    <row r="95" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="95" s="2">
       <c r="A95" s="1" t="inlineStr">
         <is>
           <t>Contested Marks(O)</t>
@@ -61469,11 +61751,14 @@
       <c r="HD95" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="HE95" t="n">
+      <c r="HE95" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="HF95" t="n">
+        <v>21</v>
+      </c>
     </row>
-    <row r="96" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="96" s="2">
       <c r="A96" s="1" t="inlineStr">
         <is>
           <t>Marks Inside 50(O)</t>
@@ -62112,11 +62397,14 @@
       <c r="HD96" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HE96" t="n">
+      <c r="HE96" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="HF96" t="n">
+        <v>19</v>
+      </c>
     </row>
-    <row r="97" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="97" s="2">
       <c r="A97" s="1" t="inlineStr">
         <is>
           <t>Clearances2(O)</t>
@@ -62755,11 +63043,14 @@
       <c r="HD97" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="HE97" t="n">
+      <c r="HE97" s="1" t="n">
         <v>38</v>
       </c>
+      <c r="HF97" t="n">
+        <v>31</v>
+      </c>
     </row>
-    <row r="98" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="98" s="2">
       <c r="A98" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s2(O)</t>
@@ -63398,11 +63689,14 @@
       <c r="HD98" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HE98" t="n">
+      <c r="HE98" s="1" t="n">
         <v>24</v>
       </c>
+      <c r="HF98" t="n">
+        <v>21</v>
+      </c>
     </row>
-    <row r="99" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="99" s="2">
       <c r="A99" s="1" t="inlineStr">
         <is>
           <t>1%ers(O)</t>
@@ -64041,11 +64335,14 @@
       <c r="HD99" s="1" t="n">
         <v>45</v>
       </c>
-      <c r="HE99" t="n">
+      <c r="HE99" s="1" t="n">
         <v>36</v>
       </c>
+      <c r="HF99" t="n">
+        <v>42</v>
+      </c>
     </row>
-    <row r="100" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="100" s="2">
       <c r="A100" s="1" t="inlineStr">
         <is>
           <t>Bounces(O)</t>
@@ -64684,11 +64981,14 @@
       <c r="HD100" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HE100" t="n">
+      <c r="HE100" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="HF100" t="n">
+        <v>3</v>
+      </c>
     </row>
-    <row r="101" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="101" s="2">
       <c r="A101" s="1" t="inlineStr">
         <is>
           <t>Goals Assists2(O)</t>
@@ -65327,11 +65627,14 @@
       <c r="HD101" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HE101" t="n">
+      <c r="HE101" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="HF101" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row r="102" ht="13.8" customHeight="1" s="2">
+    <row customHeight="1" ht="13.8" r="102" s="2">
       <c r="A102" s="1" t="inlineStr">
         <is>
           <t>Goal Assist %(O)</t>
@@ -65970,13 +66273,16 @@
       <c r="HD102" s="1" t="n">
         <v>52.9</v>
       </c>
-      <c r="HE102" t="n">
+      <c r="HE102" s="1" t="n">
         <v>58.3</v>
+      </c>
+      <c r="HF102" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added optimisation and updated to round 5
</commit_message>
<xml_diff>
--- a/Adelaide_stats.xlsx
+++ b/Adelaide_stats.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HF102"/>
+  <dimension ref="A1:HG102"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="GZ1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="HA23" activeCellId="0" pane="topLeft" sqref="HA23"/>
@@ -1030,8 +1030,11 @@
       <c r="HE1" s="1" t="n">
         <v>10141</v>
       </c>
-      <c r="HF1" t="n">
+      <c r="HF1" s="1" t="n">
         <v>10150</v>
+      </c>
+      <c r="HG1" t="n">
+        <v>10188</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="2" s="2">
@@ -1676,7 +1679,10 @@
       <c r="HE2" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="HF2" t="n">
+      <c r="HF2" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="HG2" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -2322,8 +2328,11 @@
       <c r="HE3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HF3" t="n">
+      <c r="HF3" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HG3" t="n">
+        <v>5</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="4" s="2">
@@ -2968,8 +2977,11 @@
       <c r="HE4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HF4" t="n">
+      <c r="HF4" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HG4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="5" s="2">
@@ -3614,8 +3626,11 @@
       <c r="HE5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HF5" t="n">
+      <c r="HF5" s="1" t="n">
         <v>0</v>
+      </c>
+      <c r="HG5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="6" s="2">
@@ -4260,8 +4275,11 @@
       <c r="HE6" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="HF6" t="n">
+      <c r="HF6" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="HG6" t="n">
+        <v>34</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="7" s="2">
@@ -4906,8 +4924,11 @@
       <c r="HE7" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="HF7" t="n">
+      <c r="HF7" s="1" t="n">
         <v>83</v>
+      </c>
+      <c r="HG7" t="n">
+        <v>54</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="8" s="2">
@@ -5552,8 +5573,11 @@
       <c r="HE8" s="1" t="n">
         <v>-53</v>
       </c>
-      <c r="HF8" t="n">
+      <c r="HF8" s="1" t="n">
         <v>-37</v>
+      </c>
+      <c r="HG8" t="n">
+        <v>-20</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="9" s="2">
@@ -6198,7 +6222,10 @@
       <c r="HE9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HF9" t="n">
+      <c r="HF9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HG9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6844,8 +6871,11 @@
       <c r="HE10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HF10" t="n">
+      <c r="HF10" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HG10" t="n">
+        <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="11" s="2">
@@ -7490,8 +7520,11 @@
       <c r="HE11" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="HF11" t="n">
+      <c r="HF11" s="1" t="n">
         <v>162</v>
+      </c>
+      <c r="HG11" t="n">
+        <v>170</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="12" s="2">
@@ -8136,8 +8169,11 @@
       <c r="HE12" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="HF12" t="n">
+      <c r="HF12" s="1" t="n">
         <v>70</v>
+      </c>
+      <c r="HG12" t="n">
+        <v>133</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="13" s="2">
@@ -8782,8 +8818,11 @@
       <c r="HE13" s="1" t="n">
         <v>250</v>
       </c>
-      <c r="HF13" t="n">
+      <c r="HF13" s="1" t="n">
         <v>232</v>
+      </c>
+      <c r="HG13" t="n">
+        <v>303</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="14" s="2">
@@ -9428,8 +9467,11 @@
       <c r="HE14" s="1" t="n">
         <v>1.38</v>
       </c>
-      <c r="HF14" t="n">
+      <c r="HF14" s="1" t="n">
         <v>2.31</v>
+      </c>
+      <c r="HG14" t="n">
+        <v>1.28</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="15" s="2">
@@ -10074,8 +10116,11 @@
       <c r="HE15" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="HF15" t="n">
+      <c r="HF15" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="HG15" t="n">
+        <v>79</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="16" s="2">
@@ -10720,8 +10765,11 @@
       <c r="HE16" s="1" t="n">
         <v>57</v>
       </c>
-      <c r="HF16" t="n">
+      <c r="HF16" s="1" t="n">
         <v>55</v>
+      </c>
+      <c r="HG16" t="n">
+        <v>39</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="17" s="2">
@@ -11366,8 +11414,11 @@
       <c r="HE17" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="HF17" t="n">
+      <c r="HF17" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="HG17" t="n">
+        <v>18</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="18" s="2">
@@ -12012,8 +12063,11 @@
       <c r="HE18" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="HF18" t="n">
+      <c r="HF18" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="HG18" t="n">
+        <v>13</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="19" s="2">
@@ -12658,8 +12712,11 @@
       <c r="HE19" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="HF19" t="n">
+      <c r="HF19" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HG19" t="n">
+        <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="20" s="2">
@@ -13304,8 +13361,11 @@
       <c r="HE20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HF20" t="n">
+      <c r="HF20" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HG20" t="n">
+        <v>4</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="21" s="2">
@@ -13950,8 +14010,11 @@
       <c r="HE21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HF21" t="n">
+      <c r="HF21" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HG21" t="n">
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="22" s="2">
@@ -14596,8 +14659,11 @@
       <c r="HE22" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HF22" t="n">
+      <c r="HF22" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HG22" t="n">
+        <v>7</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="23" s="2">
@@ -15242,7 +15308,10 @@
       <c r="HE23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HF23" t="n">
+      <c r="HF23" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="HG23" t="n">
         <v>3</v>
       </c>
     </row>
@@ -15888,8 +15957,11 @@
       <c r="HE24" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HF24" t="n">
+      <c r="HF24" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HG24" t="n">
+        <v>14</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="25" s="2">
@@ -16534,8 +16606,11 @@
       <c r="HE25" s="1" t="n">
         <v>44.4</v>
       </c>
-      <c r="HF25" t="n">
+      <c r="HF25" s="1" t="n">
         <v>63.6</v>
+      </c>
+      <c r="HG25" t="n">
+        <v>28.6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="26" s="2">
@@ -17180,8 +17255,11 @@
       <c r="HE26" s="1" t="n">
         <v>62.5</v>
       </c>
-      <c r="HF26" t="n">
+      <c r="HF26" s="1" t="n">
         <v>33.14</v>
+      </c>
+      <c r="HG26" t="n">
+        <v>75.75</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="27" s="2">
@@ -17826,8 +17904,11 @@
       <c r="HE27" s="1" t="n">
         <v>27.78</v>
       </c>
-      <c r="HF27" t="n">
+      <c r="HF27" s="1" t="n">
         <v>21.09</v>
+      </c>
+      <c r="HG27" t="n">
+        <v>21.64</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="28" s="2">
@@ -18472,8 +18553,11 @@
       <c r="HE28" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HF28" t="n">
+      <c r="HF28" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="HG28" t="n">
+        <v>24</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="29" s="2">
@@ -19118,8 +19202,11 @@
       <c r="HE29" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="HF29" t="n">
+      <c r="HF29" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="HG29" t="n">
+        <v>40</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="30" s="2">
@@ -19764,8 +19851,11 @@
       <c r="HE30" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="HF30" t="n">
+      <c r="HF30" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="HG30" t="n">
+        <v>33</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="31" s="2">
@@ -20410,8 +20500,11 @@
       <c r="HE31" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HF31" t="n">
+      <c r="HF31" s="1" t="n">
         <v>28</v>
+      </c>
+      <c r="HG31" t="n">
+        <v>42</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="32" s="2">
@@ -21056,8 +21149,11 @@
       <c r="HE32" s="1" t="n">
         <v>3.11</v>
       </c>
-      <c r="HF32" t="n">
+      <c r="HF32" s="1" t="n">
         <v>2.55</v>
+      </c>
+      <c r="HG32" t="n">
+        <v>3</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="33" s="2">
@@ -21702,8 +21798,11 @@
       <c r="HE33" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HF33" t="n">
+      <c r="HF33" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HG33" t="n">
+        <v>10.5</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="34" s="2">
@@ -22348,8 +22447,11 @@
       <c r="HE34" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HF34" t="n">
+      <c r="HF34" s="1" t="n">
         <v>28.6</v>
+      </c>
+      <c r="HG34" t="n">
+        <v>26.2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="35" s="2">
@@ -22994,8 +23096,11 @@
       <c r="HE35" s="1" t="n">
         <v>14.3</v>
       </c>
-      <c r="HF35" t="n">
+      <c r="HF35" s="1" t="n">
         <v>25</v>
+      </c>
+      <c r="HG35" t="n">
+        <v>9.5</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="36" s="2">
@@ -23640,8 +23745,11 @@
       <c r="HE36" s="1" t="n">
         <v>187.3</v>
       </c>
-      <c r="HF36" t="n">
+      <c r="HF36" s="1" t="n">
         <v>187.9</v>
+      </c>
+      <c r="HG36" t="n">
+        <v>187</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="37" s="2">
@@ -24286,8 +24394,11 @@
       <c r="HE37" s="1" t="n">
         <v>85.8</v>
       </c>
-      <c r="HF37" t="n">
+      <c r="HF37" s="1" t="n">
         <v>86</v>
+      </c>
+      <c r="HG37" t="n">
+        <v>85.59999999999999</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="38" s="2">
@@ -24932,8 +25043,11 @@
       <c r="HE38" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HF38" t="n">
+      <c r="HF38" s="1" t="n">
         <v>24.66</v>
+      </c>
+      <c r="HG38" t="n">
+        <v>25.24</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="39" s="2">
@@ -25578,8 +25692,11 @@
       <c r="HE39" s="1" t="n">
         <v>84</v>
       </c>
-      <c r="HF39" t="n">
+      <c r="HF39" s="1" t="n">
         <v>71</v>
+      </c>
+      <c r="HG39" t="n">
+        <v>81</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="40" s="2">
@@ -26224,8 +26341,11 @@
       <c r="HE40" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HF40" t="n">
+      <c r="HF40" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="HG40" t="n">
+        <v>11</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="41" s="2">
@@ -26870,7 +26990,10 @@
       <c r="HE41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HF41" t="n">
+      <c r="HF41" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HG41" t="n">
         <v>2</v>
       </c>
     </row>
@@ -27516,8 +27639,11 @@
       <c r="HE42" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HF42" t="n">
+      <c r="HF42" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HG42" t="n">
+        <v>4</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="43" s="2">
@@ -28162,7 +28288,10 @@
       <c r="HE43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HF43" t="n">
+      <c r="HF43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HG43" t="n">
         <v>5</v>
       </c>
     </row>
@@ -28808,8 +28937,11 @@
       <c r="HE44" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="HF44" t="n">
+      <c r="HF44" s="1" t="n">
         <v>91</v>
+      </c>
+      <c r="HG44" t="n">
+        <v>106</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="45" s="2">
@@ -29454,8 +29586,11 @@
       <c r="HE45" s="1" t="n">
         <v>143</v>
       </c>
-      <c r="HF45" t="n">
+      <c r="HF45" s="1" t="n">
         <v>125</v>
+      </c>
+      <c r="HG45" t="n">
+        <v>194</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="46" s="2">
@@ -30100,8 +30235,11 @@
       <c r="HE46" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="HF46" t="n">
+      <c r="HF46" s="1" t="n">
         <v>166</v>
+      </c>
+      <c r="HG46" t="n">
+        <v>228</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="47" s="2">
@@ -30746,8 +30884,11 @@
       <c r="HE47" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="HF47" t="n">
+      <c r="HF47" s="1" t="n">
         <v>71.59999999999999</v>
+      </c>
+      <c r="HG47" t="n">
+        <v>75.2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="48" s="2">
@@ -31392,8 +31533,11 @@
       <c r="HE48" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="HF48" t="n">
+      <c r="HF48" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="HG48" t="n">
+        <v>40</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="49" s="2">
@@ -32038,8 +32182,11 @@
       <c r="HE49" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HF49" t="n">
+      <c r="HF49" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HG49" t="n">
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="50" s="2">
@@ -32684,8 +32831,11 @@
       <c r="HE50" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HF50" t="n">
+      <c r="HF50" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HG50" t="n">
+        <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="51" s="2">
@@ -33330,8 +33480,11 @@
       <c r="HE51" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HF51" t="n">
+      <c r="HF51" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="HG51" t="n">
+        <v>24</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="52" s="2">
@@ -33976,8 +34129,11 @@
       <c r="HE52" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="HF52" t="n">
+      <c r="HF52" s="1" t="n">
         <v>46</v>
+      </c>
+      <c r="HG52" t="n">
+        <v>33</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="53" s="2">
@@ -34622,8 +34778,11 @@
       <c r="HE53" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="HF53" t="n">
+      <c r="HF53" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="HG53" t="n">
+        <v>32</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="54" s="2">
@@ -35268,8 +35427,11 @@
       <c r="HE54" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HF54" t="n">
+      <c r="HF54" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HG54" t="n">
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="55" s="2">
@@ -35914,8 +36076,11 @@
       <c r="HE55" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HF55" t="n">
+      <c r="HF55" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HG55" t="n">
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="56" s="2">
@@ -36560,8 +36725,11 @@
       <c r="HE56" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HF56" t="n">
+      <c r="HF56" s="1" t="n">
         <v>71.40000000000001</v>
+      </c>
+      <c r="HG56" t="n">
+        <v>50</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="57" s="2">
@@ -37206,8 +37374,11 @@
       <c r="HE57" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="HF57" t="n">
+      <c r="HF57" s="1" t="n">
         <v>199</v>
+      </c>
+      <c r="HG57" t="n">
+        <v>197</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="58" s="2">
@@ -37852,8 +38023,11 @@
       <c r="HE58" s="1" t="n">
         <v>123</v>
       </c>
-      <c r="HF58" t="n">
+      <c r="HF58" s="1" t="n">
         <v>86</v>
+      </c>
+      <c r="HG58" t="n">
+        <v>88</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="59" s="2">
@@ -38498,7 +38672,10 @@
       <c r="HE59" s="1" t="n">
         <v>318</v>
       </c>
-      <c r="HF59" t="n">
+      <c r="HF59" s="1" t="n">
+        <v>285</v>
+      </c>
+      <c r="HG59" t="n">
         <v>285</v>
       </c>
     </row>
@@ -39144,8 +39321,11 @@
       <c r="HE60" s="1" t="n">
         <v>1.59</v>
       </c>
-      <c r="HF60" t="n">
+      <c r="HF60" s="1" t="n">
         <v>2.31</v>
+      </c>
+      <c r="HG60" t="n">
+        <v>2.24</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="61" s="2">
@@ -39790,8 +39970,11 @@
       <c r="HE61" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="HF61" t="n">
+      <c r="HF61" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="HG61" t="n">
+        <v>109</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="62" s="2">
@@ -40436,8 +40619,11 @@
       <c r="HE62" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="HF62" t="n">
+      <c r="HF62" s="1" t="n">
         <v>68</v>
+      </c>
+      <c r="HG62" t="n">
+        <v>41</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="63" s="2">
@@ -41082,8 +41268,11 @@
       <c r="HE63" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="HF63" t="n">
+      <c r="HF63" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="HG63" t="n">
+        <v>31</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="64" s="2">
@@ -41728,8 +41917,11 @@
       <c r="HE64" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="HF64" t="n">
+      <c r="HF64" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HG64" t="n">
+        <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="65" s="2">
@@ -42374,8 +42566,11 @@
       <c r="HE65" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="HF65" t="n">
+      <c r="HF65" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="HG65" t="n">
+        <v>13</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="66" s="2">
@@ -43020,8 +43215,11 @@
       <c r="HE66" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HF66" t="n">
+      <c r="HF66" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HG66" t="n">
+        <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="67" s="2">
@@ -43666,8 +43864,11 @@
       <c r="HE67" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HF67" t="n">
+      <c r="HF67" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HG67" t="n">
+        <v>7</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="68" s="2">
@@ -44312,8 +44513,11 @@
       <c r="HE68" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HF68" t="n">
+      <c r="HF68" s="1" t="n">
         <v>22</v>
+      </c>
+      <c r="HG68" t="n">
+        <v>5</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="69" s="2">
@@ -44958,7 +45162,10 @@
       <c r="HE69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HF69" t="n">
+      <c r="HF69" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HG69" t="n">
         <v>1</v>
       </c>
     </row>
@@ -45604,8 +45811,11 @@
       <c r="HE70" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="HF70" t="n">
+      <c r="HF70" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="HG70" t="n">
+        <v>14</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="71" s="2">
@@ -46250,8 +46460,11 @@
       <c r="HE71" s="1" t="n">
         <v>54.5</v>
       </c>
-      <c r="HF71" t="n">
+      <c r="HF71" s="1" t="n">
         <v>30.3</v>
+      </c>
+      <c r="HG71" t="n">
+        <v>57.1</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="72" s="2">
@@ -46896,8 +47109,11 @@
       <c r="HE72" s="1" t="n">
         <v>26.5</v>
       </c>
-      <c r="HF72" t="n">
+      <c r="HF72" s="1" t="n">
         <v>28.5</v>
+      </c>
+      <c r="HG72" t="n">
+        <v>35.62</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="73" s="2">
@@ -47542,8 +47758,11 @@
       <c r="HE73" s="1" t="n">
         <v>14.45</v>
       </c>
-      <c r="HF73" t="n">
+      <c r="HF73" s="1" t="n">
         <v>8.640000000000001</v>
+      </c>
+      <c r="HG73" t="n">
+        <v>20.36</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="74" s="2">
@@ -48188,8 +48407,11 @@
       <c r="HE74" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="HF74" t="n">
+      <c r="HF74" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="HG74" t="n">
+        <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="75" s="2">
@@ -48834,8 +49056,11 @@
       <c r="HE75" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="HF75" t="n">
+      <c r="HF75" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="HG75" t="n">
+        <v>40</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="76" s="2">
@@ -49480,8 +49705,11 @@
       <c r="HE76" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="HF76" t="n">
+      <c r="HF76" s="1" t="n">
         <v>21</v>
+      </c>
+      <c r="HG76" t="n">
+        <v>37</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="77" s="2">
@@ -50126,8 +50354,11 @@
       <c r="HE77" s="1" t="n">
         <v>56</v>
       </c>
-      <c r="HF77" t="n">
+      <c r="HF77" s="1" t="n">
         <v>60</v>
+      </c>
+      <c r="HG77" t="n">
+        <v>43</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="78" s="2">
@@ -50772,8 +51003,11 @@
       <c r="HE78" s="1" t="n">
         <v>2.55</v>
       </c>
-      <c r="HF78" t="n">
+      <c r="HF78" s="1" t="n">
         <v>1.82</v>
+      </c>
+      <c r="HG78" t="n">
+        <v>3.07</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="79" s="2">
@@ -51418,8 +51652,11 @@
       <c r="HE79" s="1" t="n">
         <v>4.67</v>
       </c>
-      <c r="HF79" t="n">
+      <c r="HF79" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HG79" t="n">
+        <v>5.38</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="80" s="2">
@@ -52064,8 +52301,11 @@
       <c r="HE80" s="1" t="n">
         <v>37.5</v>
       </c>
-      <c r="HF80" t="n">
+      <c r="HF80" s="1" t="n">
         <v>53.3</v>
+      </c>
+      <c r="HG80" t="n">
+        <v>30.2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="81" s="2">
@@ -52710,8 +52950,11 @@
       <c r="HE81" s="1" t="n">
         <v>21.4</v>
       </c>
-      <c r="HF81" t="n">
+      <c r="HF81" s="1" t="n">
         <v>16.7</v>
+      </c>
+      <c r="HG81" t="n">
+        <v>18.6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="82" s="2">
@@ -53356,8 +53599,11 @@
       <c r="HE82" s="1" t="n">
         <v>186.9</v>
       </c>
-      <c r="HF82" t="n">
+      <c r="HF82" s="1" t="n">
         <v>188.9</v>
+      </c>
+      <c r="HG82" t="n">
+        <v>188.1</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="83" s="2">
@@ -54002,8 +54248,11 @@
       <c r="HE83" s="1" t="n">
         <v>85.3</v>
       </c>
-      <c r="HF83" t="n">
+      <c r="HF83" s="1" t="n">
         <v>89</v>
+      </c>
+      <c r="HG83" t="n">
+        <v>87.90000000000001</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="84" s="2">
@@ -54648,8 +54897,11 @@
       <c r="HE84" s="1" t="n">
         <v>24.33</v>
       </c>
-      <c r="HF84" t="n">
+      <c r="HF84" s="1" t="n">
         <v>25.66</v>
+      </c>
+      <c r="HG84" t="n">
+        <v>24.66</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="85" s="2">
@@ -55294,8 +55546,11 @@
       <c r="HE85" s="1" t="n">
         <v>74.2</v>
       </c>
-      <c r="HF85" t="n">
+      <c r="HF85" s="1" t="n">
         <v>98.5</v>
+      </c>
+      <c r="HG85" t="n">
+        <v>75.8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="86" s="2">
@@ -55940,8 +56195,11 @@
       <c r="HE86" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HF86" t="n">
+      <c r="HF86" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HG86" t="n">
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="87" s="2">
@@ -56586,8 +56844,11 @@
       <c r="HE87" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HF87" t="n">
+      <c r="HF87" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HG87" t="n">
+        <v>7</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="88" s="2">
@@ -57232,8 +57493,11 @@
       <c r="HE88" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HF88" t="n">
+      <c r="HF88" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HG88" t="n">
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="89" s="2">
@@ -57878,8 +58142,11 @@
       <c r="HE89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HF89" t="n">
+      <c r="HF89" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HG89" t="n">
+        <v>3</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="90" s="2">
@@ -58524,8 +58791,11 @@
       <c r="HE90" s="1" t="n">
         <v>122</v>
       </c>
-      <c r="HF90" t="n">
+      <c r="HF90" s="1" t="n">
         <v>131</v>
+      </c>
+      <c r="HG90" t="n">
+        <v>98</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="91" s="2">
@@ -59170,8 +59440,11 @@
       <c r="HE91" s="1" t="n">
         <v>192</v>
       </c>
-      <c r="HF91" t="n">
+      <c r="HF91" s="1" t="n">
         <v>145</v>
+      </c>
+      <c r="HG91" t="n">
+        <v>183</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="92" s="2">
@@ -59816,8 +60089,11 @@
       <c r="HE92" s="1" t="n">
         <v>227</v>
       </c>
-      <c r="HF92" t="n">
+      <c r="HF92" s="1" t="n">
         <v>190</v>
+      </c>
+      <c r="HG92" t="n">
+        <v>228</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="93" s="2">
@@ -60462,8 +60738,11 @@
       <c r="HE93" s="1" t="n">
         <v>71.40000000000001</v>
       </c>
-      <c r="HF93" t="n">
+      <c r="HF93" s="1" t="n">
         <v>66.7</v>
+      </c>
+      <c r="HG93" t="n">
+        <v>80</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="94" s="2">
@@ -61108,8 +61387,11 @@
       <c r="HE94" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="HF94" t="n">
+      <c r="HF94" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="HG94" t="n">
+        <v>40</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="95" s="2">
@@ -61754,8 +62036,11 @@
       <c r="HE95" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HF95" t="n">
+      <c r="HF95" s="1" t="n">
         <v>21</v>
+      </c>
+      <c r="HG95" t="n">
+        <v>11</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="96" s="2">
@@ -62400,8 +62685,11 @@
       <c r="HE96" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HF96" t="n">
+      <c r="HF96" s="1" t="n">
         <v>19</v>
+      </c>
+      <c r="HG96" t="n">
+        <v>15</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="97" s="2">
@@ -63046,8 +63334,11 @@
       <c r="HE97" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="HF97" t="n">
+      <c r="HF97" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="HG97" t="n">
+        <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="98" s="2">
@@ -63692,8 +63983,11 @@
       <c r="HE98" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="HF98" t="n">
+      <c r="HF98" s="1" t="n">
         <v>21</v>
+      </c>
+      <c r="HG98" t="n">
+        <v>37</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="99" s="2">
@@ -64338,8 +64632,11 @@
       <c r="HE99" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="HF99" t="n">
+      <c r="HF99" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HG99" t="n">
+        <v>29</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="100" s="2">
@@ -64984,8 +65281,11 @@
       <c r="HE100" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HF100" t="n">
+      <c r="HF100" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HG100" t="n">
+        <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="101" s="2">
@@ -65630,8 +65930,11 @@
       <c r="HE101" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HF101" t="n">
+      <c r="HF101" s="1" t="n">
         <v>9</v>
+      </c>
+      <c r="HG101" t="n">
+        <v>7</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="102" s="2">
@@ -66276,8 +66579,11 @@
       <c r="HE102" s="1" t="n">
         <v>58.3</v>
       </c>
-      <c r="HF102" t="n">
+      <c r="HF102" s="1" t="n">
         <v>90</v>
+      </c>
+      <c r="HG102" t="n">
+        <v>87.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update functions and not reset stat dataframe
</commit_message>
<xml_diff>
--- a/Adelaide_stats.xlsx
+++ b/Adelaide_stats.xlsx
@@ -377,7 +377,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HG102"/>
+  <dimension ref="A1:HJ102"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="GZ1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="HA23" activeCellId="0" pane="topLeft" sqref="HA23"/>
@@ -1033,8 +1033,17 @@
       <c r="HF1" s="1" t="n">
         <v>10150</v>
       </c>
-      <c r="HG1" t="n">
+      <c r="HG1" s="1" t="n">
         <v>10188</v>
+      </c>
+      <c r="HH1" s="1" t="n">
+        <v>10212</v>
+      </c>
+      <c r="HI1" s="1" t="n">
+        <v>10226</v>
+      </c>
+      <c r="HJ1" t="n">
+        <v>10232</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="2" s="2">
@@ -1682,7 +1691,16 @@
       <c r="HF2" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="HG2" t="n">
+      <c r="HG2" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="HH2" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="HI2" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="HJ2" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -2331,8 +2349,17 @@
       <c r="HF3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HG3" t="n">
+      <c r="HG3" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HH3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HI3" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="HJ3" t="n">
+        <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="4" s="2">
@@ -2980,7 +3007,16 @@
       <c r="HF4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HG4" t="n">
+      <c r="HG4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HH4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HI4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HJ4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3629,7 +3665,16 @@
       <c r="HF5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HG5" t="n">
+      <c r="HG5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HH5" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HI5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HJ5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -4278,8 +4323,17 @@
       <c r="HF6" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="HG6" t="n">
+      <c r="HG6" s="1" t="n">
         <v>34</v>
+      </c>
+      <c r="HH6" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="HI6" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="HJ6" t="n">
+        <v>59</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="7" s="2">
@@ -4927,8 +4981,17 @@
       <c r="HF7" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="HG7" t="n">
+      <c r="HG7" s="1" t="n">
         <v>54</v>
+      </c>
+      <c r="HH7" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="HI7" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="HJ7" t="n">
+        <v>62</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="8" s="2">
@@ -5576,8 +5639,17 @@
       <c r="HF8" s="1" t="n">
         <v>-37</v>
       </c>
-      <c r="HG8" t="n">
+      <c r="HG8" s="1" t="n">
         <v>-20</v>
+      </c>
+      <c r="HH8" s="1" t="n">
+        <v>-33</v>
+      </c>
+      <c r="HI8" s="1" t="n">
+        <v>-23</v>
+      </c>
+      <c r="HJ8" t="n">
+        <v>-3</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="9" s="2">
@@ -6225,7 +6297,16 @@
       <c r="HF9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HG9" t="n">
+      <c r="HG9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HH9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HI9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HJ9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6874,8 +6955,17 @@
       <c r="HF10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HG10" t="n">
+      <c r="HG10" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HH10" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="HI10" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="HJ10" t="n">
+        <v>5</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="11" s="2">
@@ -7523,8 +7613,17 @@
       <c r="HF11" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="HG11" t="n">
+      <c r="HG11" s="1" t="n">
         <v>170</v>
+      </c>
+      <c r="HH11" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="HI11" s="1" t="n">
+        <v>166</v>
+      </c>
+      <c r="HJ11" t="n">
+        <v>167</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="12" s="2">
@@ -8172,8 +8271,17 @@
       <c r="HF12" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="HG12" t="n">
+      <c r="HG12" s="1" t="n">
         <v>133</v>
+      </c>
+      <c r="HH12" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="HI12" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="HJ12" t="n">
+        <v>150</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="13" s="2">
@@ -8821,8 +8929,17 @@
       <c r="HF13" s="1" t="n">
         <v>232</v>
       </c>
-      <c r="HG13" t="n">
+      <c r="HG13" s="1" t="n">
         <v>303</v>
+      </c>
+      <c r="HH13" s="1" t="n">
+        <v>324</v>
+      </c>
+      <c r="HI13" s="1" t="n">
+        <v>286</v>
+      </c>
+      <c r="HJ13" t="n">
+        <v>317</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="14" s="2">
@@ -9470,8 +9587,17 @@
       <c r="HF14" s="1" t="n">
         <v>2.31</v>
       </c>
-      <c r="HG14" t="n">
+      <c r="HG14" s="1" t="n">
         <v>1.28</v>
+      </c>
+      <c r="HH14" s="1" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="HI14" s="1" t="n">
+        <v>1.38</v>
+      </c>
+      <c r="HJ14" t="n">
+        <v>1.11</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="15" s="2">
@@ -10119,8 +10245,17 @@
       <c r="HF15" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="HG15" t="n">
+      <c r="HG15" s="1" t="n">
         <v>79</v>
+      </c>
+      <c r="HH15" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="HI15" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="HJ15" t="n">
+        <v>55</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="16" s="2">
@@ -10768,8 +10903,17 @@
       <c r="HF16" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HG16" t="n">
+      <c r="HG16" s="1" t="n">
         <v>39</v>
+      </c>
+      <c r="HH16" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="HI16" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="HJ16" t="n">
+        <v>54</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="17" s="2">
@@ -11417,8 +11561,17 @@
       <c r="HF17" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="HG17" t="n">
+      <c r="HG17" s="1" t="n">
         <v>18</v>
+      </c>
+      <c r="HH17" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="HI17" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="HJ17" t="n">
+        <v>27</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="18" s="2">
@@ -12066,8 +12219,17 @@
       <c r="HF18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="HG18" t="n">
+      <c r="HG18" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="HH18" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="HI18" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="HJ18" t="n">
+        <v>16</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="19" s="2">
@@ -12715,8 +12877,17 @@
       <c r="HF19" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HG19" t="n">
+      <c r="HG19" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="HH19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="HI19" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="HJ19" t="n">
+        <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="20" s="2">
@@ -13364,8 +13535,17 @@
       <c r="HF20" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HG20" t="n">
+      <c r="HG20" s="1" t="n">
         <v>4</v>
+      </c>
+      <c r="HH20" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HI20" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="HJ20" t="n">
+        <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="21" s="2">
@@ -14013,8 +14193,17 @@
       <c r="HF21" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HG21" t="n">
+      <c r="HG21" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HH21" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="HI21" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HJ21" t="n">
+        <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="22" s="2">
@@ -14662,8 +14851,17 @@
       <c r="HF22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HG22" t="n">
+      <c r="HG22" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HH22" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="HI22" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HJ22" t="n">
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="23" s="2">
@@ -15311,8 +15509,17 @@
       <c r="HF23" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HG23" t="n">
+      <c r="HG23" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HH23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HI23" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HJ23" t="n">
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="24" s="2">
@@ -15960,8 +16167,17 @@
       <c r="HF24" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="HG24" t="n">
+      <c r="HG24" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HH24" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="HI24" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="HJ24" t="n">
+        <v>19</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="25" s="2">
@@ -16609,8 +16825,17 @@
       <c r="HF25" s="1" t="n">
         <v>63.6</v>
       </c>
-      <c r="HG25" t="n">
+      <c r="HG25" s="1" t="n">
         <v>28.6</v>
+      </c>
+      <c r="HH25" s="1" t="n">
+        <v>55.6</v>
+      </c>
+      <c r="HI25" s="1" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="HJ25" t="n">
+        <v>42.1</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="26" s="2">
@@ -17258,8 +17483,17 @@
       <c r="HF26" s="1" t="n">
         <v>33.14</v>
       </c>
-      <c r="HG26" t="n">
+      <c r="HG26" s="1" t="n">
         <v>75.75</v>
+      </c>
+      <c r="HH26" s="1" t="n">
+        <v>64.8</v>
+      </c>
+      <c r="HI26" s="1" t="n">
+        <v>35.75</v>
+      </c>
+      <c r="HJ26" t="n">
+        <v>39.62</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="27" s="2">
@@ -17907,8 +18141,17 @@
       <c r="HF27" s="1" t="n">
         <v>21.09</v>
       </c>
-      <c r="HG27" t="n">
+      <c r="HG27" s="1" t="n">
         <v>21.64</v>
+      </c>
+      <c r="HH27" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="HI27" s="1" t="n">
+        <v>19.07</v>
+      </c>
+      <c r="HJ27" t="n">
+        <v>16.68</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="28" s="2">
@@ -18556,8 +18799,17 @@
       <c r="HF28" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="HG28" t="n">
+      <c r="HG28" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="HH28" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="HI28" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="HJ28" t="n">
+        <v>29</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="29" s="2">
@@ -19205,8 +19457,17 @@
       <c r="HF29" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HG29" t="n">
+      <c r="HG29" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="HH29" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="HI29" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="HJ29" t="n">
+        <v>52</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="30" s="2">
@@ -19854,8 +20115,17 @@
       <c r="HF30" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="HG30" t="n">
+      <c r="HG30" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="HH30" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="HI30" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="HJ30" t="n">
+        <v>38</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="31" s="2">
@@ -20503,8 +20773,17 @@
       <c r="HF31" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="HG31" t="n">
+      <c r="HG31" s="1" t="n">
         <v>42</v>
+      </c>
+      <c r="HH31" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="HI31" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="HJ31" t="n">
+        <v>45</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="32" s="2">
@@ -21152,8 +21431,17 @@
       <c r="HF32" s="1" t="n">
         <v>2.55</v>
       </c>
-      <c r="HG32" t="n">
+      <c r="HG32" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HH32" s="1" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="HI32" s="1" t="n">
+        <v>2.67</v>
+      </c>
+      <c r="HJ32" t="n">
+        <v>2.37</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="33" s="2">
@@ -21801,8 +22089,17 @@
       <c r="HF33" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HG33" t="n">
+      <c r="HG33" s="1" t="n">
         <v>10.5</v>
+      </c>
+      <c r="HH33" s="1" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="HI33" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HJ33" t="n">
+        <v>5.62</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="34" s="2">
@@ -22450,8 +22747,17 @@
       <c r="HF34" s="1" t="n">
         <v>28.6</v>
       </c>
-      <c r="HG34" t="n">
+      <c r="HG34" s="1" t="n">
         <v>26.2</v>
+      </c>
+      <c r="HH34" s="1" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="HI34" s="1" t="n">
+        <v>32.5</v>
+      </c>
+      <c r="HJ34" t="n">
+        <v>40</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="35" s="2">
@@ -23099,8 +23405,17 @@
       <c r="HF35" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HG35" t="n">
+      <c r="HG35" s="1" t="n">
         <v>9.5</v>
+      </c>
+      <c r="HH35" s="1" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="HI35" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="HJ35" t="n">
+        <v>17.8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="36" s="2">
@@ -23748,7 +24063,16 @@
       <c r="HF36" s="1" t="n">
         <v>187.9</v>
       </c>
-      <c r="HG36" t="n">
+      <c r="HG36" s="1" t="n">
+        <v>187</v>
+      </c>
+      <c r="HH36" s="1" t="n">
+        <v>186.7</v>
+      </c>
+      <c r="HI36" s="1" t="n">
+        <v>186.8</v>
+      </c>
+      <c r="HJ36" t="n">
         <v>187</v>
       </c>
     </row>
@@ -24397,8 +24721,17 @@
       <c r="HF37" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="HG37" t="n">
+      <c r="HG37" s="1" t="n">
         <v>85.59999999999999</v>
+      </c>
+      <c r="HH37" s="1" t="n">
+        <v>84.5</v>
+      </c>
+      <c r="HI37" s="1" t="n">
+        <v>85.09999999999999</v>
+      </c>
+      <c r="HJ37" t="n">
+        <v>85.7</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="38" s="2">
@@ -25046,7 +25379,16 @@
       <c r="HF38" s="1" t="n">
         <v>24.66</v>
       </c>
-      <c r="HG38" t="n">
+      <c r="HG38" s="1" t="n">
+        <v>25.24</v>
+      </c>
+      <c r="HH38" s="1" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="HI38" s="1" t="n">
+        <v>25.33</v>
+      </c>
+      <c r="HJ38" t="n">
         <v>25.24</v>
       </c>
     </row>
@@ -25695,8 +26037,17 @@
       <c r="HF39" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="HG39" t="n">
+      <c r="HG39" s="1" t="n">
         <v>81</v>
+      </c>
+      <c r="HH39" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="HI39" s="1" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="HJ39" t="n">
+        <v>84</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="40" s="2">
@@ -26344,7 +26695,16 @@
       <c r="HF40" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HG40" t="n">
+      <c r="HG40" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="HH40" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="HI40" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="HJ40" t="n">
         <v>11</v>
       </c>
     </row>
@@ -26993,8 +27353,17 @@
       <c r="HF41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HG41" t="n">
+      <c r="HG41" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HH41" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HI41" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HJ41" t="n">
+        <v>1</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="42" s="2">
@@ -27642,7 +28011,16 @@
       <c r="HF42" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HG42" t="n">
+      <c r="HG42" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="HH42" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="HI42" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="HJ42" t="n">
         <v>4</v>
       </c>
     </row>
@@ -28291,8 +28669,17 @@
       <c r="HF43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HG43" t="n">
+      <c r="HG43" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HH43" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HI43" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HJ43" t="n">
+        <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="44" s="2">
@@ -28940,8 +29327,17 @@
       <c r="HF44" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="HG44" t="n">
+      <c r="HG44" s="1" t="n">
         <v>106</v>
+      </c>
+      <c r="HH44" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="HI44" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="HJ44" t="n">
+        <v>131</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="45" s="2">
@@ -29589,8 +29985,17 @@
       <c r="HF45" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="HG45" t="n">
+      <c r="HG45" s="1" t="n">
         <v>194</v>
+      </c>
+      <c r="HH45" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="HI45" s="1" t="n">
+        <v>165</v>
+      </c>
+      <c r="HJ45" t="n">
+        <v>187</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="46" s="2">
@@ -30238,8 +30643,17 @@
       <c r="HF46" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="HG46" t="n">
+      <c r="HG46" s="1" t="n">
         <v>228</v>
+      </c>
+      <c r="HH46" s="1" t="n">
+        <v>248</v>
+      </c>
+      <c r="HI46" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="HJ46" t="n">
+        <v>236</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="47" s="2">
@@ -30887,8 +31301,17 @@
       <c r="HF47" s="1" t="n">
         <v>71.59999999999999</v>
       </c>
-      <c r="HG47" t="n">
+      <c r="HG47" s="1" t="n">
         <v>75.2</v>
+      </c>
+      <c r="HH47" s="1" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="HI47" s="1" t="n">
+        <v>71.3</v>
+      </c>
+      <c r="HJ47" t="n">
+        <v>74.40000000000001</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="48" s="2">
@@ -31536,8 +31959,17 @@
       <c r="HF48" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HG48" t="n">
+      <c r="HG48" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="HH48" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="HI48" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="HJ48" t="n">
+        <v>52</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="49" s="2">
@@ -32185,8 +32617,17 @@
       <c r="HF49" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HG49" t="n">
+      <c r="HG49" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HH49" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="HI49" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="HJ49" t="n">
+        <v>11</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="50" s="2">
@@ -32834,8 +33275,17 @@
       <c r="HF50" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HG50" t="n">
+      <c r="HG50" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HH50" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="HI50" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HJ50" t="n">
+        <v>4</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="51" s="2">
@@ -33483,8 +33933,17 @@
       <c r="HF51" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="HG51" t="n">
+      <c r="HG51" s="1" t="n">
         <v>24</v>
+      </c>
+      <c r="HH51" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="HI51" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="HJ51" t="n">
+        <v>29</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="52" s="2">
@@ -34132,8 +34591,17 @@
       <c r="HF52" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="HG52" t="n">
+      <c r="HG52" s="1" t="n">
         <v>33</v>
+      </c>
+      <c r="HH52" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="HI52" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="HJ52" t="n">
+        <v>38</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="53" s="2">
@@ -34781,8 +35249,17 @@
       <c r="HF53" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="HG53" t="n">
+      <c r="HG53" s="1" t="n">
         <v>32</v>
+      </c>
+      <c r="HH53" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="HI53" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="HJ53" t="n">
+        <v>53</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="54" s="2">
@@ -35430,8 +35907,17 @@
       <c r="HF54" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HG54" t="n">
+      <c r="HG54" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HH54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="HI54" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HJ54" t="n">
+        <v>4</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="55" s="2">
@@ -36079,8 +36565,17 @@
       <c r="HF55" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HG55" t="n">
+      <c r="HG55" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HH55" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="HI55" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HJ55" t="n">
+        <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="56" s="2">
@@ -36728,8 +37223,17 @@
       <c r="HF56" s="1" t="n">
         <v>71.40000000000001</v>
       </c>
-      <c r="HG56" t="n">
+      <c r="HG56" s="1" t="n">
         <v>50</v>
+      </c>
+      <c r="HH56" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="HI56" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="HJ56" t="n">
+        <v>75</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="57" s="2">
@@ -37377,8 +37881,17 @@
       <c r="HF57" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="HG57" t="n">
+      <c r="HG57" s="1" t="n">
         <v>197</v>
+      </c>
+      <c r="HH57" s="1" t="n">
+        <v>180</v>
+      </c>
+      <c r="HI57" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="HJ57" t="n">
+        <v>176</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="58" s="2">
@@ -38026,8 +38539,17 @@
       <c r="HF58" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="HG58" t="n">
+      <c r="HG58" s="1" t="n">
         <v>88</v>
+      </c>
+      <c r="HH58" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="HI58" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="HJ58" t="n">
+        <v>146</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="59" s="2">
@@ -38675,8 +39197,17 @@
       <c r="HF59" s="1" t="n">
         <v>285</v>
       </c>
-      <c r="HG59" t="n">
+      <c r="HG59" s="1" t="n">
         <v>285</v>
+      </c>
+      <c r="HH59" s="1" t="n">
+        <v>284</v>
+      </c>
+      <c r="HI59" s="1" t="n">
+        <v>257</v>
+      </c>
+      <c r="HJ59" t="n">
+        <v>322</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="60" s="2">
@@ -39324,8 +39855,17 @@
       <c r="HF60" s="1" t="n">
         <v>2.31</v>
       </c>
-      <c r="HG60" t="n">
+      <c r="HG60" s="1" t="n">
         <v>2.24</v>
+      </c>
+      <c r="HH60" s="1" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="HI60" s="1" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="HJ60" t="n">
+        <v>1.21</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="61" s="2">
@@ -39973,8 +40513,17 @@
       <c r="HF61" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="HG61" t="n">
+      <c r="HG61" s="1" t="n">
         <v>109</v>
+      </c>
+      <c r="HH61" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="HI61" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="HJ61" t="n">
+        <v>66</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="62" s="2">
@@ -40622,8 +41171,17 @@
       <c r="HF62" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="HG62" t="n">
+      <c r="HG62" s="1" t="n">
         <v>41</v>
+      </c>
+      <c r="HH62" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="HI62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="HJ62" t="n">
+        <v>76</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="63" s="2">
@@ -41271,8 +41829,17 @@
       <c r="HF63" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="HG63" t="n">
+      <c r="HG63" s="1" t="n">
         <v>31</v>
+      </c>
+      <c r="HH63" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="HI63" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="HJ63" t="n">
+        <v>25</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="64" s="2">
@@ -41920,8 +42487,17 @@
       <c r="HF64" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HG64" t="n">
+      <c r="HG64" s="1" t="n">
         <v>17</v>
+      </c>
+      <c r="HH64" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="HI64" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="HJ64" t="n">
+        <v>20</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="65" s="2">
@@ -42569,8 +43145,17 @@
       <c r="HF65" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="HG65" t="n">
+      <c r="HG65" s="1" t="n">
         <v>13</v>
+      </c>
+      <c r="HH65" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="HI65" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="HJ65" t="n">
+        <v>16</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="66" s="2">
@@ -43218,8 +43803,17 @@
       <c r="HF66" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HG66" t="n">
+      <c r="HG66" s="1" t="n">
         <v>8</v>
+      </c>
+      <c r="HH66" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="HI66" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="HJ66" t="n">
+        <v>9</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="67" s="2">
@@ -43867,8 +44461,17 @@
       <c r="HF67" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HG67" t="n">
+      <c r="HG67" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HH67" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HI67" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HJ67" t="n">
+        <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="68" s="2">
@@ -44516,8 +45119,17 @@
       <c r="HF68" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="HG68" t="n">
+      <c r="HG68" s="1" t="n">
         <v>5</v>
+      </c>
+      <c r="HH68" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="HI68" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="HJ68" t="n">
+        <v>6</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="69" s="2">
@@ -45165,8 +45777,17 @@
       <c r="HF69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HG69" t="n">
+      <c r="HG69" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="HH69" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HI69" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="HJ69" t="n">
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="70" s="2">
@@ -45814,8 +46435,17 @@
       <c r="HF70" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="HG70" t="n">
+      <c r="HG70" s="1" t="n">
         <v>14</v>
+      </c>
+      <c r="HH70" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="HI70" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="HJ70" t="n">
+        <v>17</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="71" s="2">
@@ -46463,8 +47093,17 @@
       <c r="HF71" s="1" t="n">
         <v>30.3</v>
       </c>
-      <c r="HG71" t="n">
+      <c r="HG71" s="1" t="n">
         <v>57.1</v>
+      </c>
+      <c r="HH71" s="1" t="n">
+        <v>58.8</v>
+      </c>
+      <c r="HI71" s="1" t="n">
+        <v>66.7</v>
+      </c>
+      <c r="HJ71" t="n">
+        <v>52.9</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="72" s="2">
@@ -47112,8 +47751,17 @@
       <c r="HF72" s="1" t="n">
         <v>28.5</v>
       </c>
-      <c r="HG72" t="n">
+      <c r="HG72" s="1" t="n">
         <v>35.62</v>
+      </c>
+      <c r="HH72" s="1" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="HI72" s="1" t="n">
+        <v>21.42</v>
+      </c>
+      <c r="HJ72" t="n">
+        <v>35.78</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="73" s="2">
@@ -47761,8 +48409,17 @@
       <c r="HF73" s="1" t="n">
         <v>8.640000000000001</v>
       </c>
-      <c r="HG73" t="n">
+      <c r="HG73" s="1" t="n">
         <v>20.36</v>
+      </c>
+      <c r="HH73" s="1" t="n">
+        <v>16.71</v>
+      </c>
+      <c r="HI73" s="1" t="n">
+        <v>14.28</v>
+      </c>
+      <c r="HJ73" t="n">
+        <v>18.94</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="74" s="2">
@@ -48410,8 +49067,17 @@
       <c r="HF74" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HG74" t="n">
+      <c r="HG74" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HH74" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="HI74" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="HJ74" t="n">
+        <v>37</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="75" s="2">
@@ -49059,8 +49725,17 @@
       <c r="HF75" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="HG75" t="n">
+      <c r="HG75" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="HH75" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="HI75" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="HJ75" t="n">
+        <v>64</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="76" s="2">
@@ -49708,7 +50383,16 @@
       <c r="HF76" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="HG76" t="n">
+      <c r="HG76" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="HH76" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="HI76" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="HJ76" t="n">
         <v>37</v>
       </c>
     </row>
@@ -50357,8 +51041,17 @@
       <c r="HF77" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HG77" t="n">
+      <c r="HG77" s="1" t="n">
         <v>43</v>
+      </c>
+      <c r="HH77" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="HI77" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="HJ77" t="n">
+        <v>47</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="78" s="2">
@@ -51006,8 +51699,17 @@
       <c r="HF78" s="1" t="n">
         <v>1.82</v>
       </c>
-      <c r="HG78" t="n">
+      <c r="HG78" s="1" t="n">
         <v>3.07</v>
+      </c>
+      <c r="HH78" s="1" t="n">
+        <v>2.88</v>
+      </c>
+      <c r="HI78" s="1" t="n">
+        <v>1.94</v>
+      </c>
+      <c r="HJ78" t="n">
+        <v>2.76</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="79" s="2">
@@ -51655,8 +52357,17 @@
       <c r="HF79" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HG79" t="n">
+      <c r="HG79" s="1" t="n">
         <v>5.38</v>
+      </c>
+      <c r="HH79" s="1" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="HI79" s="1" t="n">
+        <v>2.92</v>
+      </c>
+      <c r="HJ79" t="n">
+        <v>5.22</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="80" s="2">
@@ -52304,8 +53015,17 @@
       <c r="HF80" s="1" t="n">
         <v>53.3</v>
       </c>
-      <c r="HG80" t="n">
+      <c r="HG80" s="1" t="n">
         <v>30.2</v>
+      </c>
+      <c r="HH80" s="1" t="n">
+        <v>34.7</v>
+      </c>
+      <c r="HI80" s="1" t="n">
+        <v>42.9</v>
+      </c>
+      <c r="HJ80" t="n">
+        <v>31.9</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="81" s="2">
@@ -52953,8 +53673,17 @@
       <c r="HF81" s="1" t="n">
         <v>16.7</v>
       </c>
-      <c r="HG81" t="n">
+      <c r="HG81" s="1" t="n">
         <v>18.6</v>
+      </c>
+      <c r="HH81" s="1" t="n">
+        <v>20.4</v>
+      </c>
+      <c r="HI81" s="1" t="n">
+        <v>34.3</v>
+      </c>
+      <c r="HJ81" t="n">
+        <v>19.1</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="82" s="2">
@@ -53602,8 +54331,17 @@
       <c r="HF82" s="1" t="n">
         <v>188.9</v>
       </c>
-      <c r="HG82" t="n">
+      <c r="HG82" s="1" t="n">
         <v>188.1</v>
+      </c>
+      <c r="HH82" s="1" t="n">
+        <v>188.2</v>
+      </c>
+      <c r="HI82" s="1" t="n">
+        <v>188</v>
+      </c>
+      <c r="HJ82" t="n">
+        <v>185.1</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="83" s="2">
@@ -54251,8 +54989,17 @@
       <c r="HF83" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="HG83" t="n">
+      <c r="HG83" s="1" t="n">
         <v>87.90000000000001</v>
+      </c>
+      <c r="HH83" s="1" t="n">
+        <v>87.8</v>
+      </c>
+      <c r="HI83" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="HJ83" t="n">
+        <v>85</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="84" s="2">
@@ -54900,8 +55647,17 @@
       <c r="HF84" s="1" t="n">
         <v>25.66</v>
       </c>
-      <c r="HG84" t="n">
+      <c r="HG84" s="1" t="n">
         <v>24.66</v>
+      </c>
+      <c r="HH84" s="1" t="n">
+        <v>26.24</v>
+      </c>
+      <c r="HI84" s="1" t="n">
+        <v>24.74</v>
+      </c>
+      <c r="HJ84" t="n">
+        <v>25.8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="85" s="2">
@@ -55549,8 +56305,17 @@
       <c r="HF85" s="1" t="n">
         <v>98.5</v>
       </c>
-      <c r="HG85" t="n">
+      <c r="HG85" s="1" t="n">
         <v>75.8</v>
+      </c>
+      <c r="HH85" s="1" t="n">
+        <v>115.6</v>
+      </c>
+      <c r="HI85" s="1" t="n">
+        <v>81.5</v>
+      </c>
+      <c r="HJ85" t="n">
+        <v>76.5</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="86" s="2">
@@ -56198,8 +56963,17 @@
       <c r="HF86" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HG86" t="n">
+      <c r="HG86" s="1" t="n">
         <v>10</v>
+      </c>
+      <c r="HH86" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="HI86" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="HJ86" t="n">
+        <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="87" s="2">
@@ -56847,8 +57621,17 @@
       <c r="HF87" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HG87" t="n">
+      <c r="HG87" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HH87" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="HI87" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="HJ87" t="n">
+        <v>9</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="88" s="2">
@@ -57496,8 +58279,17 @@
       <c r="HF88" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HG88" t="n">
+      <c r="HG88" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="HH88" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HI88" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="HJ88" t="n">
+        <v>3</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="89" s="2">
@@ -58145,8 +58937,17 @@
       <c r="HF89" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HG89" t="n">
+      <c r="HG89" s="1" t="n">
         <v>3</v>
+      </c>
+      <c r="HH89" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="HI89" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="HJ89" t="n">
+        <v>2</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="90" s="2">
@@ -58794,8 +59595,17 @@
       <c r="HF90" s="1" t="n">
         <v>131</v>
       </c>
-      <c r="HG90" t="n">
+      <c r="HG90" s="1" t="n">
         <v>98</v>
+      </c>
+      <c r="HH90" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="HI90" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="HJ90" t="n">
+        <v>138</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="91" s="2">
@@ -59443,8 +60253,17 @@
       <c r="HF91" s="1" t="n">
         <v>145</v>
       </c>
-      <c r="HG91" t="n">
+      <c r="HG91" s="1" t="n">
         <v>183</v>
+      </c>
+      <c r="HH91" s="1" t="n">
+        <v>190</v>
+      </c>
+      <c r="HI91" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="HJ91" t="n">
+        <v>175</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="92" s="2">
@@ -60092,8 +60911,17 @@
       <c r="HF92" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="HG92" t="n">
+      <c r="HG92" s="1" t="n">
         <v>228</v>
+      </c>
+      <c r="HH92" s="1" t="n">
+        <v>219</v>
+      </c>
+      <c r="HI92" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="HJ92" t="n">
+        <v>220</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="93" s="2">
@@ -60741,8 +61569,17 @@
       <c r="HF93" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="HG93" t="n">
+      <c r="HG93" s="1" t="n">
         <v>80</v>
+      </c>
+      <c r="HH93" s="1" t="n">
+        <v>77.09999999999999</v>
+      </c>
+      <c r="HI93" s="1" t="n">
+        <v>68.09999999999999</v>
+      </c>
+      <c r="HJ93" t="n">
+        <v>68.3</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="94" s="2">
@@ -61390,8 +62227,17 @@
       <c r="HF94" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="HG94" t="n">
+      <c r="HG94" s="1" t="n">
         <v>40</v>
+      </c>
+      <c r="HH94" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="HI94" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="HJ94" t="n">
+        <v>64</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="95" s="2">
@@ -62039,8 +62885,17 @@
       <c r="HF95" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="HG95" t="n">
+      <c r="HG95" s="1" t="n">
         <v>11</v>
+      </c>
+      <c r="HH95" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="HI95" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="HJ95" t="n">
+        <v>10</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="96" s="2">
@@ -62688,8 +63543,17 @@
       <c r="HF96" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="HG96" t="n">
+      <c r="HG96" s="1" t="n">
         <v>15</v>
+      </c>
+      <c r="HH96" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="HI96" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="HJ96" t="n">
+        <v>4</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="97" s="2">
@@ -63337,8 +64201,17 @@
       <c r="HF97" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HG97" t="n">
+      <c r="HG97" s="1" t="n">
         <v>20</v>
+      </c>
+      <c r="HH97" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="HI97" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="HJ97" t="n">
+        <v>37</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="98" s="2">
@@ -63986,7 +64859,16 @@
       <c r="HF98" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="HG98" t="n">
+      <c r="HG98" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="HH98" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="HI98" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="HJ98" t="n">
         <v>37</v>
       </c>
     </row>
@@ -64635,8 +65517,17 @@
       <c r="HF99" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="HG99" t="n">
+      <c r="HG99" s="1" t="n">
         <v>29</v>
+      </c>
+      <c r="HH99" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="HI99" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="HJ99" t="n">
+        <v>41</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="100" s="2">
@@ -65284,8 +66175,17 @@
       <c r="HF100" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HG100" t="n">
+      <c r="HG100" s="1" t="n">
         <v>6</v>
+      </c>
+      <c r="HH100" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="HI100" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="HJ100" t="n">
+        <v>9</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="101" s="2">
@@ -65933,8 +66833,17 @@
       <c r="HF101" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HG101" t="n">
+      <c r="HG101" s="1" t="n">
         <v>7</v>
+      </c>
+      <c r="HH101" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HI101" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="HJ101" t="n">
+        <v>8</v>
       </c>
     </row>
     <row customHeight="1" ht="13.8" r="102" s="2">
@@ -66582,8 +67491,17 @@
       <c r="HF102" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="HG102" t="n">
+      <c r="HG102" s="1" t="n">
         <v>87.5</v>
+      </c>
+      <c r="HH102" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="HI102" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="HJ102" t="n">
+        <v>88.90000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All games up to round 9 2020 in system
</commit_message>
<xml_diff>
--- a/Adelaide_stats.xlsx
+++ b/Adelaide_stats.xlsx
@@ -4,13 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.0001" refMode="A1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -59,31 +59,31 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" name="Comma" xfId="1"/>
-    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
-    <cellStyle builtinId="4" name="Currency" xfId="3"/>
-    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
-    <cellStyle builtinId="5" name="Percent" xfId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -377,18 +377,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:HJ102"/>
+  <dimension ref="A1:HK102"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="GZ1" view="normal" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="HA23" activeCellId="0" pane="topLeft" sqref="HA23"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="GZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="HA23" activeCellId="0" sqref="HA23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col customWidth="1" max="1025" min="1" style="1" width="8.529999999999999"/>
+    <col width="8.529999999999999" customWidth="1" style="1" min="1" max="1025"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="13.8" r="1" s="2">
+    <row r="1" ht="13.8" customHeight="1" s="2">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Match_ID</t>
@@ -1042,11 +1042,14 @@
       <c r="HI1" s="1" t="n">
         <v>10226</v>
       </c>
-      <c r="HJ1" t="n">
+      <c r="HJ1" s="1" t="n">
         <v>10232</v>
       </c>
+      <c r="HK1" t="n">
+        <v>10240</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="2" s="2">
+    <row r="2" ht="13.8" customHeight="1" s="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Year</t>
@@ -1700,11 +1703,14 @@
       <c r="HI2" s="1" t="n">
         <v>2020</v>
       </c>
-      <c r="HJ2" t="n">
+      <c r="HJ2" s="1" t="n">
         <v>2020</v>
       </c>
+      <c r="HK2" t="n">
+        <v>2020</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="3" s="2">
+    <row r="3" ht="13.8" customHeight="1" s="2">
       <c r="A3" s="1" t="inlineStr">
         <is>
           <t>Round</t>
@@ -2358,11 +2364,14 @@
       <c r="HI3" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="HJ3" t="n">
+      <c r="HJ3" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="HK3" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="4" s="2">
+    <row r="4" ht="13.8" customHeight="1" s="2">
       <c r="A4" s="1" t="inlineStr">
         <is>
           <t>H/A?</t>
@@ -3016,11 +3025,14 @@
       <c r="HI4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HJ4" t="n">
+      <c r="HJ4" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="HK4" t="n">
+        <v>1</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="5" s="2">
+    <row r="5" ht="13.8" customHeight="1" s="2">
       <c r="A5" s="1" t="inlineStr">
         <is>
           <t>H/A Win?</t>
@@ -3674,11 +3686,14 @@
       <c r="HI5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="HJ5" t="n">
+      <c r="HJ5" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="HK5" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="6" s="2">
+    <row r="6" ht="13.8" customHeight="1" s="2">
       <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Points For</t>
@@ -4332,11 +4347,14 @@
       <c r="HI6" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="HJ6" t="n">
+      <c r="HJ6" s="1" t="n">
         <v>59</v>
       </c>
+      <c r="HK6" t="n">
+        <v>50</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="7" s="2">
+    <row r="7" ht="13.8" customHeight="1" s="2">
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Points Against</t>
@@ -4990,11 +5008,14 @@
       <c r="HI7" s="1" t="n">
         <v>78</v>
       </c>
-      <c r="HJ7" t="n">
+      <c r="HJ7" s="1" t="n">
         <v>62</v>
       </c>
+      <c r="HK7" t="n">
+        <v>119</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="8" s="2">
+    <row r="8" ht="13.8" customHeight="1" s="2">
       <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Margin</t>
@@ -5648,11 +5669,14 @@
       <c r="HI8" s="1" t="n">
         <v>-23</v>
       </c>
-      <c r="HJ8" t="n">
+      <c r="HJ8" s="1" t="n">
         <v>-3</v>
       </c>
+      <c r="HK8" t="n">
+        <v>-69</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="9" s="2">
+    <row r="9" ht="13.8" customHeight="1" s="2">
       <c r="A9" s="1" t="inlineStr">
         <is>
           <t>Team Won? (1=W, 0=L)</t>
@@ -6306,11 +6330,14 @@
       <c r="HI9" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HJ9" t="n">
+      <c r="HJ9" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="HK9" t="n">
+        <v>0</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="10" s="2">
+    <row r="10" ht="13.8" customHeight="1" s="2">
       <c r="A10" s="1" t="inlineStr">
         <is>
           <t>Team_against_ID</t>
@@ -6964,11 +6991,14 @@
       <c r="HI10" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HJ10" t="n">
+      <c r="HJ10" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="HK10" t="n">
+        <v>12</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="11" s="2">
+    <row r="11" ht="13.8" customHeight="1" s="2">
       <c r="A11" s="1" t="inlineStr">
         <is>
           <t>Kicks</t>
@@ -7622,11 +7652,14 @@
       <c r="HI11" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="HJ11" t="n">
+      <c r="HJ11" s="1" t="n">
         <v>167</v>
       </c>
+      <c r="HK11" t="n">
+        <v>137</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="12" s="2">
+    <row r="12" ht="13.8" customHeight="1" s="2">
       <c r="A12" s="1" t="inlineStr">
         <is>
           <t>Handballs</t>
@@ -8280,11 +8313,14 @@
       <c r="HI12" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="HJ12" t="n">
+      <c r="HJ12" s="1" t="n">
         <v>150</v>
       </c>
+      <c r="HK12" t="n">
+        <v>121</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="13" s="2">
+    <row r="13" ht="13.8" customHeight="1" s="2">
       <c r="A13" s="1" t="inlineStr">
         <is>
           <t>Disposals</t>
@@ -8938,11 +8974,14 @@
       <c r="HI13" s="1" t="n">
         <v>286</v>
       </c>
-      <c r="HJ13" t="n">
+      <c r="HJ13" s="1" t="n">
         <v>317</v>
       </c>
+      <c r="HK13" t="n">
+        <v>258</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="14" s="2">
+    <row r="14" ht="13.8" customHeight="1" s="2">
       <c r="A14" s="1" t="inlineStr">
         <is>
           <t>Kick to HB Ratio</t>
@@ -9596,11 +9635,14 @@
       <c r="HI14" s="1" t="n">
         <v>1.38</v>
       </c>
-      <c r="HJ14" t="n">
+      <c r="HJ14" s="1" t="n">
         <v>1.11</v>
       </c>
+      <c r="HK14" t="n">
+        <v>1.13</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="15" s="2">
+    <row r="15" ht="13.8" customHeight="1" s="2">
       <c r="A15" s="1" t="inlineStr">
         <is>
           <t>Marks</t>
@@ -10254,11 +10296,14 @@
       <c r="HI15" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="HJ15" t="n">
+      <c r="HJ15" s="1" t="n">
         <v>55</v>
       </c>
+      <c r="HK15" t="n">
+        <v>53</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="16" s="2">
+    <row r="16" ht="13.8" customHeight="1" s="2">
       <c r="A16" s="1" t="inlineStr">
         <is>
           <t>Tackles</t>
@@ -10912,11 +10957,14 @@
       <c r="HI16" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="HJ16" t="n">
+      <c r="HJ16" s="1" t="n">
         <v>54</v>
       </c>
+      <c r="HK16" t="n">
+        <v>73</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="17" s="2">
+    <row r="17" ht="13.8" customHeight="1" s="2">
       <c r="A17" s="1" t="inlineStr">
         <is>
           <t>Hitouts</t>
@@ -11570,11 +11618,14 @@
       <c r="HI17" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="HJ17" t="n">
+      <c r="HJ17" s="1" t="n">
         <v>27</v>
       </c>
+      <c r="HK17" t="n">
+        <v>27</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="18" s="2">
+    <row r="18" ht="13.8" customHeight="1" s="2">
       <c r="A18" s="1" t="inlineStr">
         <is>
           <t>Frees For</t>
@@ -12228,11 +12279,14 @@
       <c r="HI18" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="HJ18" t="n">
+      <c r="HJ18" s="1" t="n">
         <v>16</v>
       </c>
+      <c r="HK18" t="n">
+        <v>22</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="19" s="2">
+    <row r="19" ht="13.8" customHeight="1" s="2">
       <c r="A19" s="1" t="inlineStr">
         <is>
           <t>Frees Against</t>
@@ -12886,11 +12940,14 @@
       <c r="HI19" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="HJ19" t="n">
+      <c r="HJ19" s="1" t="n">
         <v>20</v>
       </c>
+      <c r="HK19" t="n">
+        <v>17</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="20" s="2">
+    <row r="20" ht="13.8" customHeight="1" s="2">
       <c r="A20" s="1" t="inlineStr">
         <is>
           <t>Goals Kicked</t>
@@ -13544,11 +13601,14 @@
       <c r="HI20" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HJ20" t="n">
+      <c r="HJ20" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="HK20" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="21" s="2">
+    <row r="21" ht="13.8" customHeight="1" s="2">
       <c r="A21" s="1" t="inlineStr">
         <is>
           <t>Goal Assists1</t>
@@ -14202,11 +14262,14 @@
       <c r="HI21" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HJ21" t="n">
+      <c r="HJ21" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="HK21" t="n">
+        <v>3</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="22" s="2">
+    <row r="22" ht="13.8" customHeight="1" s="2">
       <c r="A22" s="1" t="inlineStr">
         <is>
           <t>Behinds Kicked</t>
@@ -14860,11 +14923,14 @@
       <c r="HI22" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HJ22" t="n">
+      <c r="HJ22" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="HK22" t="n">
+        <v>3</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="23" s="2">
+    <row r="23" ht="13.8" customHeight="1" s="2">
       <c r="A23" s="1" t="inlineStr">
         <is>
           <t>Rushed Behinds</t>
@@ -15518,11 +15584,14 @@
       <c r="HI23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HJ23" t="n">
+      <c r="HJ23" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="HK23" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="24" s="2">
+    <row r="24" ht="13.8" customHeight="1" s="2">
       <c r="A24" s="1" t="inlineStr">
         <is>
           <t>Scoring Shots</t>
@@ -16176,11 +16245,14 @@
       <c r="HI24" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="HJ24" t="n">
+      <c r="HJ24" s="1" t="n">
         <v>19</v>
       </c>
+      <c r="HK24" t="n">
+        <v>15</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="25" s="2">
+    <row r="25" ht="13.8" customHeight="1" s="2">
       <c r="A25" s="1" t="inlineStr">
         <is>
           <t>Conversion %</t>
@@ -16834,11 +16906,14 @@
       <c r="HI25" s="1" t="n">
         <v>53.3</v>
       </c>
-      <c r="HJ25" t="n">
+      <c r="HJ25" s="1" t="n">
         <v>42.1</v>
       </c>
+      <c r="HK25" t="n">
+        <v>46.7</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="26" s="2">
+    <row r="26" ht="13.8" customHeight="1" s="2">
       <c r="A26" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Goal</t>
@@ -17492,11 +17567,14 @@
       <c r="HI26" s="1" t="n">
         <v>35.75</v>
       </c>
-      <c r="HJ26" t="n">
+      <c r="HJ26" s="1" t="n">
         <v>39.62</v>
       </c>
+      <c r="HK26" t="n">
+        <v>36.86</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="27" s="2">
+    <row r="27" ht="13.8" customHeight="1" s="2">
       <c r="A27" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Scoring Shot</t>
@@ -18150,11 +18228,14 @@
       <c r="HI27" s="1" t="n">
         <v>19.07</v>
       </c>
-      <c r="HJ27" t="n">
+      <c r="HJ27" s="1" t="n">
         <v>16.68</v>
       </c>
+      <c r="HK27" t="n">
+        <v>17.2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="28" s="2">
+    <row r="28" ht="13.8" customHeight="1" s="2">
       <c r="A28" s="1" t="inlineStr">
         <is>
           <t>Clearances1</t>
@@ -18808,11 +18889,14 @@
       <c r="HI28" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HJ28" t="n">
+      <c r="HJ28" s="1" t="n">
         <v>29</v>
       </c>
+      <c r="HK28" t="n">
+        <v>20</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="29" s="2">
+    <row r="29" ht="13.8" customHeight="1" s="2">
       <c r="A29" s="1" t="inlineStr">
         <is>
           <t>Clangers1</t>
@@ -19466,11 +19550,14 @@
       <c r="HI29" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="HJ29" t="n">
+      <c r="HJ29" s="1" t="n">
         <v>52</v>
       </c>
+      <c r="HK29" t="n">
+        <v>47</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="30" s="2">
+    <row r="30" ht="13.8" customHeight="1" s="2">
       <c r="A30" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s1</t>
@@ -20124,11 +20211,14 @@
       <c r="HI30" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="HJ30" t="n">
+      <c r="HJ30" s="1" t="n">
         <v>38</v>
       </c>
+      <c r="HK30" t="n">
+        <v>29</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="31" s="2">
+    <row r="31" ht="13.8" customHeight="1" s="2">
       <c r="A31" s="1" t="inlineStr">
         <is>
           <t>Inside 50s</t>
@@ -20782,11 +20872,14 @@
       <c r="HI31" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="HJ31" t="n">
+      <c r="HJ31" s="1" t="n">
         <v>45</v>
       </c>
+      <c r="HK31" t="n">
+        <v>36</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="32" s="2">
+    <row r="32" ht="13.8" customHeight="1" s="2">
       <c r="A32" s="1" t="inlineStr">
         <is>
           <t>In50s Per Scoring Shot</t>
@@ -21440,11 +21533,14 @@
       <c r="HI32" s="1" t="n">
         <v>2.67</v>
       </c>
-      <c r="HJ32" t="n">
+      <c r="HJ32" s="1" t="n">
         <v>2.37</v>
       </c>
+      <c r="HK32" t="n">
+        <v>2.4</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="33" s="2">
+    <row r="33" ht="13.8" customHeight="1" s="2">
       <c r="A33" s="1" t="inlineStr">
         <is>
           <t>In50s Per Goal</t>
@@ -22098,11 +22194,14 @@
       <c r="HI33" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="HJ33" t="n">
+      <c r="HJ33" s="1" t="n">
         <v>5.62</v>
       </c>
+      <c r="HK33" t="n">
+        <v>5.14</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="34" s="2">
+    <row r="34" ht="13.8" customHeight="1" s="2">
       <c r="A34" s="1" t="inlineStr">
         <is>
           <t>% In50s Score</t>
@@ -22756,11 +22855,14 @@
       <c r="HI34" s="1" t="n">
         <v>32.5</v>
       </c>
-      <c r="HJ34" t="n">
+      <c r="HJ34" s="1" t="n">
         <v>40</v>
       </c>
+      <c r="HK34" t="n">
+        <v>27.8</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="35" s="2">
+    <row r="35" ht="13.8" customHeight="1" s="2">
       <c r="A35" s="1" t="inlineStr">
         <is>
           <t>% In50s Goal</t>
@@ -23414,11 +23516,14 @@
       <c r="HI35" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="HJ35" t="n">
+      <c r="HJ35" s="1" t="n">
         <v>17.8</v>
       </c>
+      <c r="HK35" t="n">
+        <v>19.4</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="36" s="2">
+    <row r="36" ht="13.8" customHeight="1" s="2">
       <c r="A36" s="1" t="inlineStr">
         <is>
           <t>Height</t>
@@ -24072,11 +24177,14 @@
       <c r="HI36" s="1" t="n">
         <v>186.8</v>
       </c>
-      <c r="HJ36" t="n">
+      <c r="HJ36" s="1" t="n">
         <v>187</v>
       </c>
+      <c r="HK36" t="n">
+        <v>187.2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="37" s="2">
+    <row r="37" ht="13.8" customHeight="1" s="2">
       <c r="A37" s="1" t="inlineStr">
         <is>
           <t>Weight</t>
@@ -24730,11 +24838,14 @@
       <c r="HI37" s="1" t="n">
         <v>85.09999999999999</v>
       </c>
-      <c r="HJ37" t="n">
+      <c r="HJ37" s="1" t="n">
         <v>85.7</v>
       </c>
+      <c r="HK37" t="n">
+        <v>85.3</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="38" s="2">
+    <row r="38" ht="13.8" customHeight="1" s="2">
       <c r="A38" s="1" t="inlineStr">
         <is>
           <t>Age</t>
@@ -25388,11 +25499,14 @@
       <c r="HI38" s="1" t="n">
         <v>25.33</v>
       </c>
-      <c r="HJ38" t="n">
+      <c r="HJ38" s="1" t="n">
         <v>25.24</v>
       </c>
+      <c r="HK38" t="n">
+        <v>25.33</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="39" s="2">
+    <row r="39" ht="13.8" customHeight="1" s="2">
       <c r="A39" s="1" t="inlineStr">
         <is>
           <t>Av Games</t>
@@ -26046,11 +26160,14 @@
       <c r="HI39" s="1" t="n">
         <v>84.90000000000001</v>
       </c>
-      <c r="HJ39" t="n">
+      <c r="HJ39" s="1" t="n">
         <v>84</v>
       </c>
+      <c r="HK39" t="n">
+        <v>83</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="40" s="2">
+    <row r="40" ht="13.8" customHeight="1" s="2">
       <c r="A40" s="1" t="inlineStr">
         <is>
           <t>&lt;50 Games</t>
@@ -26704,11 +26821,14 @@
       <c r="HI40" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="HJ40" t="n">
+      <c r="HJ40" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="HK40" t="n">
+        <v>10</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="41" s="2">
+    <row r="41" ht="13.8" customHeight="1" s="2">
       <c r="A41" s="1" t="inlineStr">
         <is>
           <t>50-99 Games</t>
@@ -27362,11 +27482,14 @@
       <c r="HI41" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HJ41" t="n">
+      <c r="HJ41" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="HK41" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="42" s="2">
+    <row r="42" ht="13.8" customHeight="1" s="2">
       <c r="A42" s="1" t="inlineStr">
         <is>
           <t>100-149 Games</t>
@@ -28020,11 +28143,14 @@
       <c r="HI42" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HJ42" t="n">
+      <c r="HJ42" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="HK42" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="43" s="2">
+    <row r="43" ht="13.8" customHeight="1" s="2">
       <c r="A43" s="1" t="inlineStr">
         <is>
           <t>&gt;150 Games</t>
@@ -28678,11 +28804,14 @@
       <c r="HI43" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HJ43" t="n">
+      <c r="HJ43" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="HK43" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="44" s="2">
+    <row r="44" ht="13.8" customHeight="1" s="2">
       <c r="A44" s="1" t="inlineStr">
         <is>
           <t>Contested Poss</t>
@@ -29336,11 +29465,14 @@
       <c r="HI44" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="HJ44" t="n">
+      <c r="HJ44" s="1" t="n">
         <v>131</v>
       </c>
+      <c r="HK44" t="n">
+        <v>102</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="45" s="2">
+    <row r="45" ht="13.8" customHeight="1" s="2">
       <c r="A45" s="1" t="inlineStr">
         <is>
           <t>Uncontested Poss</t>
@@ -29994,11 +30126,14 @@
       <c r="HI45" s="1" t="n">
         <v>165</v>
       </c>
-      <c r="HJ45" t="n">
+      <c r="HJ45" s="1" t="n">
         <v>187</v>
       </c>
+      <c r="HK45" t="n">
+        <v>155</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="46" s="2">
+    <row r="46" ht="13.8" customHeight="1" s="2">
       <c r="A46" s="1" t="inlineStr">
         <is>
           <t>Effective Disposals</t>
@@ -30652,11 +30787,14 @@
       <c r="HI46" s="1" t="n">
         <v>204</v>
       </c>
-      <c r="HJ46" t="n">
+      <c r="HJ46" s="1" t="n">
         <v>236</v>
       </c>
+      <c r="HK46" t="n">
+        <v>185</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="47" s="2">
+    <row r="47" ht="13.8" customHeight="1" s="2">
       <c r="A47" s="1" t="inlineStr">
         <is>
           <t>Disposal Efficiency</t>
@@ -31310,11 +31448,14 @@
       <c r="HI47" s="1" t="n">
         <v>71.3</v>
       </c>
-      <c r="HJ47" t="n">
+      <c r="HJ47" s="1" t="n">
         <v>74.40000000000001</v>
       </c>
+      <c r="HK47" t="n">
+        <v>71.7</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="48" s="2">
+    <row r="48" ht="13.8" customHeight="1" s="2">
       <c r="A48" s="1" t="inlineStr">
         <is>
           <t>Clangers2</t>
@@ -31968,11 +32109,14 @@
       <c r="HI48" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="HJ48" t="n">
+      <c r="HJ48" s="1" t="n">
         <v>52</v>
       </c>
+      <c r="HK48" t="n">
+        <v>47</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="49" s="2">
+    <row r="49" ht="13.8" customHeight="1" s="2">
       <c r="A49" s="1" t="inlineStr">
         <is>
           <t>Contested Marks</t>
@@ -32626,11 +32770,14 @@
       <c r="HI49" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="HJ49" t="n">
+      <c r="HJ49" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="HK49" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="50" s="2">
+    <row r="50" ht="13.8" customHeight="1" s="2">
       <c r="A50" s="1" t="inlineStr">
         <is>
           <t>Marks Inside 50</t>
@@ -33284,11 +33431,14 @@
       <c r="HI50" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HJ50" t="n">
+      <c r="HJ50" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="HK50" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="51" s="2">
+    <row r="51" ht="13.8" customHeight="1" s="2">
       <c r="A51" s="1" t="inlineStr">
         <is>
           <t>Clearances2</t>
@@ -33942,11 +34092,14 @@
       <c r="HI51" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HJ51" t="n">
+      <c r="HJ51" s="1" t="n">
         <v>29</v>
       </c>
+      <c r="HK51" t="n">
+        <v>20</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="52" s="2">
+    <row r="52" ht="13.8" customHeight="1" s="2">
       <c r="A52" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s2</t>
@@ -34600,11 +34753,14 @@
       <c r="HI52" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="HJ52" t="n">
+      <c r="HJ52" s="1" t="n">
         <v>38</v>
       </c>
+      <c r="HK52" t="n">
+        <v>29</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="53" s="2">
+    <row r="53" ht="13.8" customHeight="1" s="2">
       <c r="A53" s="1" t="inlineStr">
         <is>
           <t>1%ers</t>
@@ -35258,11 +35414,14 @@
       <c r="HI53" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="HJ53" t="n">
+      <c r="HJ53" s="1" t="n">
         <v>53</v>
       </c>
+      <c r="HK53" t="n">
+        <v>38</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="54" s="2">
+    <row r="54" ht="13.8" customHeight="1" s="2">
       <c r="A54" s="1" t="inlineStr">
         <is>
           <t>Bounces</t>
@@ -35916,11 +36075,14 @@
       <c r="HI54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HJ54" t="n">
+      <c r="HJ54" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="HK54" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="55" s="2">
+    <row r="55" ht="13.8" customHeight="1" s="2">
       <c r="A55" s="1" t="inlineStr">
         <is>
           <t>Goals Assists2</t>
@@ -36574,11 +36736,14 @@
       <c r="HI55" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="HJ55" t="n">
+      <c r="HJ55" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="HK55" t="n">
+        <v>3</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="56" s="2">
+    <row r="56" ht="13.8" customHeight="1" s="2">
       <c r="A56" s="1" t="inlineStr">
         <is>
           <t>Goal Assist %</t>
@@ -37232,11 +37397,14 @@
       <c r="HI56" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="HJ56" t="n">
+      <c r="HJ56" s="1" t="n">
         <v>75</v>
       </c>
+      <c r="HK56" t="n">
+        <v>42.9</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="57" s="2">
+    <row r="57" ht="13.8" customHeight="1" s="2">
       <c r="A57" s="1" t="inlineStr">
         <is>
           <t>Kicks (O)</t>
@@ -37890,11 +38058,14 @@
       <c r="HI57" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="HJ57" t="n">
+      <c r="HJ57" s="1" t="n">
         <v>176</v>
       </c>
+      <c r="HK57" t="n">
+        <v>201</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="58" s="2">
+    <row r="58" ht="13.8" customHeight="1" s="2">
       <c r="A58" s="1" t="inlineStr">
         <is>
           <t>Handballs (O)</t>
@@ -38548,11 +38719,14 @@
       <c r="HI58" s="1" t="n">
         <v>82</v>
       </c>
-      <c r="HJ58" t="n">
+      <c r="HJ58" s="1" t="n">
         <v>146</v>
       </c>
+      <c r="HK58" t="n">
+        <v>157</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="59" s="2">
+    <row r="59" ht="13.8" customHeight="1" s="2">
       <c r="A59" s="1" t="inlineStr">
         <is>
           <t>Disposals (O)</t>
@@ -39206,11 +39380,14 @@
       <c r="HI59" s="1" t="n">
         <v>257</v>
       </c>
-      <c r="HJ59" t="n">
+      <c r="HJ59" s="1" t="n">
         <v>322</v>
       </c>
+      <c r="HK59" t="n">
+        <v>358</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="60" s="2">
+    <row r="60" ht="13.8" customHeight="1" s="2">
       <c r="A60" s="1" t="inlineStr">
         <is>
           <t>Kick to HB Ratio (O)</t>
@@ -39864,11 +40041,14 @@
       <c r="HI60" s="1" t="n">
         <v>2.13</v>
       </c>
-      <c r="HJ60" t="n">
+      <c r="HJ60" s="1" t="n">
         <v>1.21</v>
       </c>
+      <c r="HK60" t="n">
+        <v>1.28</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="61" s="2">
+    <row r="61" ht="13.8" customHeight="1" s="2">
       <c r="A61" s="1" t="inlineStr">
         <is>
           <t>Marks (O)</t>
@@ -40522,11 +40702,14 @@
       <c r="HI61" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="HJ61" t="n">
+      <c r="HJ61" s="1" t="n">
         <v>66</v>
       </c>
+      <c r="HK61" t="n">
+        <v>100</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="62" s="2">
+    <row r="62" ht="13.8" customHeight="1" s="2">
       <c r="A62" s="1" t="inlineStr">
         <is>
           <t>Tackles(O)</t>
@@ -41180,11 +41363,14 @@
       <c r="HI62" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="HJ62" t="n">
+      <c r="HJ62" s="1" t="n">
         <v>76</v>
       </c>
+      <c r="HK62" t="n">
+        <v>66</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="63" s="2">
+    <row r="63" ht="13.8" customHeight="1" s="2">
       <c r="A63" s="1" t="inlineStr">
         <is>
           <t>Hitouts(O)</t>
@@ -41838,11 +42024,14 @@
       <c r="HI63" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="HJ63" t="n">
+      <c r="HJ63" s="1" t="n">
         <v>25</v>
       </c>
+      <c r="HK63" t="n">
+        <v>29</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="64" s="2">
+    <row r="64" ht="13.8" customHeight="1" s="2">
       <c r="A64" s="1" t="inlineStr">
         <is>
           <t>Frees For(O)</t>
@@ -42496,11 +42685,14 @@
       <c r="HI64" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="HJ64" t="n">
+      <c r="HJ64" s="1" t="n">
         <v>20</v>
       </c>
+      <c r="HK64" t="n">
+        <v>17</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="65" s="2">
+    <row r="65" ht="13.8" customHeight="1" s="2">
       <c r="A65" s="1" t="inlineStr">
         <is>
           <t>Frees Against(O)</t>
@@ -43154,11 +43346,14 @@
       <c r="HI65" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="HJ65" t="n">
+      <c r="HJ65" s="1" t="n">
         <v>16</v>
       </c>
+      <c r="HK65" t="n">
+        <v>22</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="66" s="2">
+    <row r="66" ht="13.8" customHeight="1" s="2">
       <c r="A66" s="1" t="inlineStr">
         <is>
           <t>Goals Kicked(O)</t>
@@ -43812,11 +44007,14 @@
       <c r="HI66" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="HJ66" t="n">
+      <c r="HJ66" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="HK66" t="n">
+        <v>19</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="67" s="2">
+    <row r="67" ht="13.8" customHeight="1" s="2">
       <c r="A67" s="1" t="inlineStr">
         <is>
           <t>Goal Assists1(O)</t>
@@ -44470,11 +44668,14 @@
       <c r="HI67" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HJ67" t="n">
+      <c r="HJ67" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="HK67" t="n">
+        <v>13</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="68" s="2">
+    <row r="68" ht="13.8" customHeight="1" s="2">
       <c r="A68" s="1" t="inlineStr">
         <is>
           <t>Behinds Kicked(O)</t>
@@ -45128,11 +45329,14 @@
       <c r="HI68" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HJ68" t="n">
+      <c r="HJ68" s="1" t="n">
         <v>6</v>
       </c>
+      <c r="HK68" t="n">
+        <v>3</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="69" s="2">
+    <row r="69" ht="13.8" customHeight="1" s="2">
       <c r="A69" s="1" t="inlineStr">
         <is>
           <t>Rushed Behinds(O)</t>
@@ -45786,11 +45990,14 @@
       <c r="HI69" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HJ69" t="n">
+      <c r="HJ69" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HK69" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="70" s="2">
+    <row r="70" ht="13.8" customHeight="1" s="2">
       <c r="A70" s="1" t="inlineStr">
         <is>
           <t>Scoring Shots(O)</t>
@@ -46444,11 +46651,14 @@
       <c r="HI70" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="HJ70" t="n">
+      <c r="HJ70" s="1" t="n">
         <v>17</v>
       </c>
+      <c r="HK70" t="n">
+        <v>24</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="71" s="2">
+    <row r="71" ht="13.8" customHeight="1" s="2">
       <c r="A71" s="1" t="inlineStr">
         <is>
           <t>Conversion %(O)</t>
@@ -47102,11 +47312,14 @@
       <c r="HI71" s="1" t="n">
         <v>66.7</v>
       </c>
-      <c r="HJ71" t="n">
+      <c r="HJ71" s="1" t="n">
         <v>52.9</v>
       </c>
+      <c r="HK71" t="n">
+        <v>79.2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="72" s="2">
+    <row r="72" ht="13.8" customHeight="1" s="2">
       <c r="A72" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Goal(O)</t>
@@ -47760,11 +47973,14 @@
       <c r="HI72" s="1" t="n">
         <v>21.42</v>
       </c>
-      <c r="HJ72" t="n">
+      <c r="HJ72" s="1" t="n">
         <v>35.78</v>
       </c>
+      <c r="HK72" t="n">
+        <v>18.84</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="73" s="2">
+    <row r="73" ht="13.8" customHeight="1" s="2">
       <c r="A73" s="1" t="inlineStr">
         <is>
           <t>Disposals Per Scoring Shot(O)</t>
@@ -48418,11 +48634,14 @@
       <c r="HI73" s="1" t="n">
         <v>14.28</v>
       </c>
-      <c r="HJ73" t="n">
+      <c r="HJ73" s="1" t="n">
         <v>18.94</v>
       </c>
+      <c r="HK73" t="n">
+        <v>14.92</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="74" s="2">
+    <row r="74" ht="13.8" customHeight="1" s="2">
       <c r="A74" s="1" t="inlineStr">
         <is>
           <t>Clearances1(O)</t>
@@ -49076,11 +49295,14 @@
       <c r="HI74" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="HJ74" t="n">
+      <c r="HJ74" s="1" t="n">
         <v>37</v>
       </c>
+      <c r="HK74" t="n">
+        <v>35</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="75" s="2">
+    <row r="75" ht="13.8" customHeight="1" s="2">
       <c r="A75" s="1" t="inlineStr">
         <is>
           <t>Clangers1(O)</t>
@@ -49734,11 +49956,14 @@
       <c r="HI75" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="HJ75" t="n">
+      <c r="HJ75" s="1" t="n">
         <v>64</v>
       </c>
+      <c r="HK75" t="n">
+        <v>53</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="76" s="2">
+    <row r="76" ht="13.8" customHeight="1" s="2">
       <c r="A76" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s1(O)</t>
@@ -50392,11 +50617,14 @@
       <c r="HI76" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HJ76" t="n">
+      <c r="HJ76" s="1" t="n">
         <v>37</v>
       </c>
+      <c r="HK76" t="n">
+        <v>28</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="77" s="2">
+    <row r="77" ht="13.8" customHeight="1" s="2">
       <c r="A77" s="1" t="inlineStr">
         <is>
           <t>Inside 50s(O)</t>
@@ -51050,11 +51278,14 @@
       <c r="HI77" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="HJ77" t="n">
+      <c r="HJ77" s="1" t="n">
         <v>47</v>
       </c>
+      <c r="HK77" t="n">
+        <v>48</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="78" s="2">
+    <row r="78" ht="13.8" customHeight="1" s="2">
       <c r="A78" s="1" t="inlineStr">
         <is>
           <t>In50s Per Scoring Shot(O)</t>
@@ -51708,11 +51939,14 @@
       <c r="HI78" s="1" t="n">
         <v>1.94</v>
       </c>
-      <c r="HJ78" t="n">
+      <c r="HJ78" s="1" t="n">
         <v>2.76</v>
       </c>
+      <c r="HK78" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="79" s="2">
+    <row r="79" ht="13.8" customHeight="1" s="2">
       <c r="A79" s="1" t="inlineStr">
         <is>
           <t>In50s Per Goal(O)</t>
@@ -52366,11 +52600,14 @@
       <c r="HI79" s="1" t="n">
         <v>2.92</v>
       </c>
-      <c r="HJ79" t="n">
+      <c r="HJ79" s="1" t="n">
         <v>5.22</v>
       </c>
+      <c r="HK79" t="n">
+        <v>2.53</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="80" s="2">
+    <row r="80" ht="13.8" customHeight="1" s="2">
       <c r="A80" s="1" t="inlineStr">
         <is>
           <t>% In50s Score(O)</t>
@@ -53024,11 +53261,14 @@
       <c r="HI80" s="1" t="n">
         <v>42.9</v>
       </c>
-      <c r="HJ80" t="n">
+      <c r="HJ80" s="1" t="n">
         <v>31.9</v>
       </c>
+      <c r="HK80" t="n">
+        <v>45.8</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="81" s="2">
+    <row r="81" ht="13.8" customHeight="1" s="2">
       <c r="A81" s="1" t="inlineStr">
         <is>
           <t>% In50s Goal(O)</t>
@@ -53682,11 +53922,14 @@
       <c r="HI81" s="1" t="n">
         <v>34.3</v>
       </c>
-      <c r="HJ81" t="n">
+      <c r="HJ81" s="1" t="n">
         <v>19.1</v>
       </c>
+      <c r="HK81" t="n">
+        <v>39.6</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="82" s="2">
+    <row r="82" ht="13.8" customHeight="1" s="2">
       <c r="A82" s="1" t="inlineStr">
         <is>
           <t>Height(O)</t>
@@ -54340,11 +54583,14 @@
       <c r="HI82" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="HJ82" t="n">
+      <c r="HJ82" s="1" t="n">
         <v>185.1</v>
       </c>
+      <c r="HK82" t="n">
+        <v>188.9</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="83" s="2">
+    <row r="83" ht="13.8" customHeight="1" s="2">
       <c r="A83" s="1" t="inlineStr">
         <is>
           <t>Weight(O)</t>
@@ -54998,11 +55244,14 @@
       <c r="HI83" s="1" t="n">
         <v>86</v>
       </c>
-      <c r="HJ83" t="n">
+      <c r="HJ83" s="1" t="n">
         <v>85</v>
       </c>
+      <c r="HK83" t="n">
+        <v>87.2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="84" s="2">
+    <row r="84" ht="13.8" customHeight="1" s="2">
       <c r="A84" s="1" t="inlineStr">
         <is>
           <t>Age(O)</t>
@@ -55656,11 +55905,14 @@
       <c r="HI84" s="1" t="n">
         <v>24.74</v>
       </c>
-      <c r="HJ84" t="n">
+      <c r="HJ84" s="1" t="n">
         <v>25.8</v>
       </c>
+      <c r="HK84" t="n">
+        <v>25.33</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="85" s="2">
+    <row r="85" ht="13.8" customHeight="1" s="2">
       <c r="A85" s="1" t="inlineStr">
         <is>
           <t>Av Games(O)</t>
@@ -56314,11 +56566,14 @@
       <c r="HI85" s="1" t="n">
         <v>81.5</v>
       </c>
-      <c r="HJ85" t="n">
+      <c r="HJ85" s="1" t="n">
         <v>76.5</v>
       </c>
+      <c r="HK85" t="n">
+        <v>86.2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="86" s="2">
+    <row r="86" ht="13.8" customHeight="1" s="2">
       <c r="A86" s="1" t="inlineStr">
         <is>
           <t>&lt;50 Games(O)</t>
@@ -56972,11 +57227,14 @@
       <c r="HI86" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HJ86" t="n">
+      <c r="HJ86" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="HK86" t="n">
+        <v>9</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="87" s="2">
+    <row r="87" ht="13.8" customHeight="1" s="2">
       <c r="A87" s="1" t="inlineStr">
         <is>
           <t>50-99 Games(O)</t>
@@ -57630,11 +57888,14 @@
       <c r="HI87" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="HJ87" t="n">
+      <c r="HJ87" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="HK87" t="n">
+        <v>5</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="88" s="2">
+    <row r="88" ht="13.8" customHeight="1" s="2">
       <c r="A88" s="1" t="inlineStr">
         <is>
           <t>100-149 Games(O)</t>
@@ -58288,11 +58549,14 @@
       <c r="HI88" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HJ88" t="n">
+      <c r="HJ88" s="1" t="n">
         <v>3</v>
       </c>
+      <c r="HK88" t="n">
+        <v>2</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="89" s="2">
+    <row r="89" ht="13.8" customHeight="1" s="2">
       <c r="A89" s="1" t="inlineStr">
         <is>
           <t>&gt;150 Games(O)</t>
@@ -58946,11 +59210,14 @@
       <c r="HI89" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="HJ89" t="n">
+      <c r="HJ89" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="HK89" t="n">
+        <v>6</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="90" s="2">
+    <row r="90" ht="13.8" customHeight="1" s="2">
       <c r="A90" s="1" t="inlineStr">
         <is>
           <t>Contested Poss(O)</t>
@@ -59604,11 +59871,14 @@
       <c r="HI90" s="1" t="n">
         <v>119</v>
       </c>
-      <c r="HJ90" t="n">
+      <c r="HJ90" s="1" t="n">
         <v>138</v>
       </c>
+      <c r="HK90" t="n">
+        <v>125</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="91" s="2">
+    <row r="91" ht="13.8" customHeight="1" s="2">
       <c r="A91" s="1" t="inlineStr">
         <is>
           <t>Uncontested Poss(O)</t>
@@ -60262,11 +60532,14 @@
       <c r="HI91" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="HJ91" t="n">
+      <c r="HJ91" s="1" t="n">
         <v>175</v>
       </c>
+      <c r="HK91" t="n">
+        <v>232</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="92" s="2">
+    <row r="92" ht="13.8" customHeight="1" s="2">
       <c r="A92" s="1" t="inlineStr">
         <is>
           <t>Effective Disposals(O)</t>
@@ -60920,11 +61193,14 @@
       <c r="HI92" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="HJ92" t="n">
+      <c r="HJ92" s="1" t="n">
         <v>220</v>
       </c>
+      <c r="HK92" t="n">
+        <v>269</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="93" s="2">
+    <row r="93" ht="13.8" customHeight="1" s="2">
       <c r="A93" s="1" t="inlineStr">
         <is>
           <t>Disposal Efficiency(O)</t>
@@ -61578,11 +61854,14 @@
       <c r="HI93" s="1" t="n">
         <v>68.09999999999999</v>
       </c>
-      <c r="HJ93" t="n">
+      <c r="HJ93" s="1" t="n">
         <v>68.3</v>
       </c>
+      <c r="HK93" t="n">
+        <v>75.09999999999999</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="94" s="2">
+    <row r="94" ht="13.8" customHeight="1" s="2">
       <c r="A94" s="1" t="inlineStr">
         <is>
           <t>Clangers2(O)</t>
@@ -62236,11 +62515,14 @@
       <c r="HI94" s="1" t="n">
         <v>59</v>
       </c>
-      <c r="HJ94" t="n">
+      <c r="HJ94" s="1" t="n">
         <v>64</v>
       </c>
+      <c r="HK94" t="n">
+        <v>53</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="95" s="2">
+    <row r="95" ht="13.8" customHeight="1" s="2">
       <c r="A95" s="1" t="inlineStr">
         <is>
           <t>Contested Marks(O)</t>
@@ -62894,11 +63176,14 @@
       <c r="HI95" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="HJ95" t="n">
+      <c r="HJ95" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="HK95" t="n">
+        <v>15</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="96" s="2">
+    <row r="96" ht="13.8" customHeight="1" s="2">
       <c r="A96" s="1" t="inlineStr">
         <is>
           <t>Marks Inside 50(O)</t>
@@ -63552,11 +63837,14 @@
       <c r="HI96" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="HJ96" t="n">
+      <c r="HJ96" s="1" t="n">
         <v>4</v>
       </c>
+      <c r="HK96" t="n">
+        <v>10</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="97" s="2">
+    <row r="97" ht="13.8" customHeight="1" s="2">
       <c r="A97" s="1" t="inlineStr">
         <is>
           <t>Clearances2(O)</t>
@@ -64210,11 +64498,14 @@
       <c r="HI97" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="HJ97" t="n">
+      <c r="HJ97" s="1" t="n">
         <v>37</v>
       </c>
+      <c r="HK97" t="n">
+        <v>35</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="98" s="2">
+    <row r="98" ht="13.8" customHeight="1" s="2">
       <c r="A98" s="1" t="inlineStr">
         <is>
           <t>Rebound 50s2(O)</t>
@@ -64868,11 +65159,14 @@
       <c r="HI98" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="HJ98" t="n">
+      <c r="HJ98" s="1" t="n">
         <v>37</v>
       </c>
+      <c r="HK98" t="n">
+        <v>28</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="99" s="2">
+    <row r="99" ht="13.8" customHeight="1" s="2">
       <c r="A99" s="1" t="inlineStr">
         <is>
           <t>1%ers(O)</t>
@@ -65526,11 +65820,14 @@
       <c r="HI99" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="HJ99" t="n">
+      <c r="HJ99" s="1" t="n">
         <v>41</v>
       </c>
+      <c r="HK99" t="n">
+        <v>33</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="100" s="2">
+    <row r="100" ht="13.8" customHeight="1" s="2">
       <c r="A100" s="1" t="inlineStr">
         <is>
           <t>Bounces(O)</t>
@@ -66184,11 +66481,14 @@
       <c r="HI100" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="HJ100" t="n">
+      <c r="HJ100" s="1" t="n">
         <v>9</v>
       </c>
+      <c r="HK100" t="n">
+        <v>7</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="101" s="2">
+    <row r="101" ht="13.8" customHeight="1" s="2">
       <c r="A101" s="1" t="inlineStr">
         <is>
           <t>Goals Assists2(O)</t>
@@ -66842,11 +67142,14 @@
       <c r="HI101" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="HJ101" t="n">
+      <c r="HJ101" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="HK101" t="n">
+        <v>13</v>
+      </c>
     </row>
-    <row customHeight="1" ht="13.8" r="102" s="2">
+    <row r="102" ht="13.8" customHeight="1" s="2">
       <c r="A102" s="1" t="inlineStr">
         <is>
           <t>Goal Assist %(O)</t>
@@ -67500,13 +67803,16 @@
       <c r="HI102" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="HJ102" t="n">
+      <c r="HJ102" s="1" t="n">
         <v>88.90000000000001</v>
+      </c>
+      <c r="HK102" t="n">
+        <v>68.40000000000001</v>
       </c>
     </row>
   </sheetData>
-  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1" footer="0.511805555555555" header="0.511805555555555" left="0.75" right="0.75" top="1"/>
-  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" verticalDpi="300"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>